<commit_message>
Subiendo Diagrama de Gantt
</commit_message>
<xml_diff>
--- a/documentación/Plantilla Diagrama de Gantt.xlsx
+++ b/documentación/Plantilla Diagrama de Gantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE9B35C-6DC3-463F-B7A4-B6C78E1EFF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F525E169-8728-4079-9A78-CF7BA83BD399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -135,9 +135,6 @@
 Aparece una barra de estado con sombreado para las fechas especificadas en bloques comenzando desde la celda I9 hasta la BL9. </t>
   </si>
   <si>
-    <t>Tarea 1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -145,18 +142,6 @@
 Repita las instrucciones de la celda A9 para todas las filas de tareas en esta hoja de cálculo. Sobrescriba los datos de ejemplo.
 Un ejemplo de otra fase empieza en la celda A14. 
 Continue escribiendo tareas en las celdas de la A10 a la A13 o vaya a la celda A14 para obtener más información.</t>
-  </si>
-  <si>
-    <t>Tarea 2</t>
-  </si>
-  <si>
-    <t>Tarea 3</t>
-  </si>
-  <si>
-    <t>Tarea 4</t>
-  </si>
-  <si>
-    <t>Tarea 5</t>
   </si>
   <si>
     <t>La celda a la derecha contiene el título de ejemplo de la Fase 2. 
@@ -169,16 +154,7 @@
 Repita las instrucciones de las celdas A8 y A9 cuando lo necesite.</t>
   </si>
   <si>
-    <t>Trabajo o fase 2</t>
-  </si>
-  <si>
     <t>Bloque de título fase de ejemplo</t>
-  </si>
-  <si>
-    <t>Trabajo o fase 3</t>
-  </si>
-  <si>
-    <t>Trabajo o fase 4</t>
   </si>
   <si>
     <t>Esta es una fila vacía.</t>
@@ -209,9 +185,6 @@
     <t>Manolo</t>
   </si>
   <si>
-    <t>Aaron y JR</t>
-  </si>
-  <si>
     <t>Juan Carlos y Iosu</t>
   </si>
   <si>
@@ -224,7 +197,115 @@
     <t>Crear app Main Scrapper</t>
   </si>
   <si>
-    <t>Clase Embedding y Clase BD</t>
+    <t>Iosu</t>
+  </si>
+  <si>
+    <t>Clase BDChoma</t>
+  </si>
+  <si>
+    <t>Web UI y LLM</t>
+  </si>
+  <si>
+    <t>BackEnd de control de usuario</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>UI de acceso (login)</t>
+  </si>
+  <si>
+    <t>Juan Carlos</t>
+  </si>
+  <si>
+    <t>UI de Registro</t>
+  </si>
+  <si>
+    <t>UI de ChatBot</t>
+  </si>
+  <si>
+    <t>LLM</t>
+  </si>
+  <si>
+    <t>Integración PDFs díarios BD</t>
+  </si>
+  <si>
+    <t>Log y Power BI</t>
+  </si>
+  <si>
+    <t>Integracición UI y LLM</t>
+  </si>
+  <si>
+    <t>JR y Juan Carlos</t>
+  </si>
+  <si>
+    <t>Clase LOGChatBOC</t>
+  </si>
+  <si>
+    <t>Iosu y Aarón</t>
+  </si>
+  <si>
+    <t>Aarón</t>
+  </si>
+  <si>
+    <t>Aarón y JR</t>
+  </si>
+  <si>
+    <t>Mejoras (Si nos da tiempo)</t>
+  </si>
+  <si>
+    <t>Inyección de LOG (ChatBoc)</t>
+  </si>
+  <si>
+    <t>Documentación</t>
+  </si>
+  <si>
+    <t>Manual de Despliegle</t>
+  </si>
+  <si>
+    <t>Manual de Implementación</t>
+  </si>
+  <si>
+    <t>Manual de Usuario</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Docker Ollama</t>
+  </si>
+  <si>
+    <t>Docker de Base de datos (User)</t>
+  </si>
+  <si>
+    <t>Docker Web y LLM</t>
+  </si>
+  <si>
+    <t>Iosu y JR</t>
+  </si>
+  <si>
+    <t>Panel de Control Power Bi</t>
+  </si>
+  <si>
+    <t>Preparación Datos Power Bi</t>
+  </si>
+  <si>
+    <t>Test Unitarios</t>
+  </si>
+  <si>
+    <t>Pruebas del sistema</t>
+  </si>
+  <si>
+    <t>JR y Aarón</t>
+  </si>
+  <si>
+    <t>App Android (Básica)</t>
+  </si>
+  <si>
+    <t>Docker API-REST</t>
+  </si>
+  <si>
+    <t>API + LLM</t>
   </si>
 </sst>
 </file>
@@ -474,7 +555,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="47">
+  <fills count="52">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -735,6 +816,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -991,7 +1102,7 @@
     <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1186,6 +1297,9 @@
     <xf numFmtId="0" fontId="0" fillId="45" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1201,8 +1315,35 @@
     <xf numFmtId="169" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="50" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="50" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="50" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="50" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="51" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="51" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="51" borderId="2" xfId="10" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1547,9 +1688,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>98220</xdr:rowOff>
+      <xdr:rowOff>94410</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1857,11 +1998,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA38"/>
+  <dimension ref="A1:AA47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1907,10 +2048,10 @@
       <c r="C3" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="70">
+      <c r="D3" s="71">
         <v>45432</v>
       </c>
-      <c r="E3" s="70"/>
+      <c r="E3" s="71"/>
     </row>
     <row r="4" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
@@ -1922,38 +2063,38 @@
       <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="H4" s="71">
+      <c r="H4" s="72">
         <f>H5</f>
         <v>45432</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="71">
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="72">
         <f>H5+7</f>
         <v>45439</v>
       </c>
-      <c r="N4" s="72"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="73">
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="74">
         <f>H5+14</f>
         <v>45446</v>
       </c>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="74"/>
-      <c r="W4" s="73">
+      <c r="S4" s="75"/>
+      <c r="T4" s="75"/>
+      <c r="U4" s="75"/>
+      <c r="V4" s="75"/>
+      <c r="W4" s="74">
         <f>H5+21</f>
         <v>45453</v>
       </c>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
+      <c r="X4" s="75"/>
+      <c r="Y4" s="75"/>
+      <c r="Z4" s="75"/>
+      <c r="AA4" s="75"/>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
@@ -2166,7 +2307,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="48"/>
@@ -2199,10 +2340,10 @@
         <v>22</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D9" s="50">
         <f>Inicio_del_proyecto</f>
@@ -2213,8 +2354,8 @@
       </c>
       <c r="F9" s="68"/>
       <c r="G9" s="68"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
       <c r="J9" s="68"/>
       <c r="K9" s="68"/>
       <c r="L9" s="68"/>
@@ -2230,7 +2371,7 @@
       <c r="V9" s="21"/>
       <c r="W9" s="21"/>
       <c r="X9" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Y9" s="21"/>
       <c r="Z9" s="21"/>
@@ -2238,13 +2379,13 @@
     </row>
     <row r="10" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D10" s="50">
         <f>Inicio_del_proyecto</f>
@@ -2255,8 +2396,8 @@
       </c>
       <c r="F10" s="67"/>
       <c r="G10" s="67"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
       <c r="J10" s="68"/>
       <c r="K10" s="68"/>
       <c r="L10" s="68"/>
@@ -2279,10 +2420,10 @@
     <row r="11" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
       <c r="B11" s="40" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D11" s="50">
         <f>Inicio_del_proyecto</f>
@@ -2291,7 +2432,7 @@
       <c r="E11" s="50"/>
       <c r="F11" s="67"/>
       <c r="G11" s="67"/>
-      <c r="H11" s="68"/>
+      <c r="H11" s="76"/>
       <c r="I11" s="68"/>
       <c r="J11" s="68"/>
       <c r="K11" s="68"/>
@@ -2315,10 +2456,10 @@
     <row r="12" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="24"/>
       <c r="B12" s="40" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D12" s="50">
         <f>Inicio_del_proyecto</f>
@@ -2327,7 +2468,7 @@
       <c r="E12" s="50"/>
       <c r="F12" s="67"/>
       <c r="G12" s="67"/>
-      <c r="H12" s="68"/>
+      <c r="H12" s="77"/>
       <c r="I12" s="68"/>
       <c r="J12" s="68"/>
       <c r="K12" s="68"/>
@@ -2351,10 +2492,10 @@
     <row r="13" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="40" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D13" s="50">
         <f>Inicio_del_proyecto</f>
@@ -2363,7 +2504,7 @@
       <c r="E13" s="50"/>
       <c r="F13" s="67"/>
       <c r="G13" s="67"/>
-      <c r="H13" s="68"/>
+      <c r="H13" s="78"/>
       <c r="I13" s="68"/>
       <c r="J13" s="68"/>
       <c r="K13" s="68"/>
@@ -2387,16 +2528,16 @@
     <row r="14" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24"/>
       <c r="B14" s="40" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
       <c r="F14" s="67"/>
       <c r="G14" s="67"/>
-      <c r="H14" s="68"/>
+      <c r="H14" s="78"/>
       <c r="I14" s="68"/>
       <c r="J14" s="68"/>
       <c r="K14" s="68"/>
@@ -2420,16 +2561,16 @@
     <row r="15" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="24"/>
       <c r="B15" s="40" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="50"/>
       <c r="E15" s="50"/>
       <c r="F15" s="67"/>
       <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
+      <c r="H15" s="78"/>
       <c r="I15" s="68"/>
       <c r="J15" s="68"/>
       <c r="K15" s="68"/>
@@ -2441,7 +2582,7 @@
       <c r="Q15" s="68"/>
       <c r="R15" s="68"/>
       <c r="S15" s="68"/>
-      <c r="T15" s="68"/>
+      <c r="T15" s="69"/>
       <c r="U15" s="21"/>
       <c r="V15" s="21"/>
       <c r="W15" s="21"/>
@@ -2451,21 +2592,18 @@
       <c r="AA15" s="21"/>
     </row>
     <row r="16" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="52"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
       <c r="F16" s="67"/>
-      <c r="G16" s="67" t="str">
-        <f t="shared" ref="G16:G35" si="3">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v/>
-      </c>
-      <c r="H16" s="68"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="77"/>
       <c r="I16" s="68"/>
       <c r="J16" s="68"/>
       <c r="K16" s="68"/>
@@ -2487,16 +2625,18 @@
       <c r="AA16" s="21"/>
     </row>
     <row r="17" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="25"/>
-      <c r="B17" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
+      <c r="A17" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="52"/>
       <c r="F17" s="67"/>
       <c r="G17" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="G17:G44" si="3">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="H17" s="68"/>
@@ -2521,11 +2661,13 @@
       <c r="AA17" s="21"/>
     </row>
     <row r="18" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="24"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="34"/>
+        <v>66</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>35</v>
+      </c>
       <c r="D18" s="53"/>
       <c r="E18" s="53"/>
       <c r="F18" s="67"/>
@@ -2555,18 +2697,17 @@
       <c r="AA18" s="21"/>
     </row>
     <row r="19" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="24"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="34"/>
+        <v>65</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>35</v>
+      </c>
       <c r="D19" s="53"/>
       <c r="E19" s="53"/>
       <c r="F19" s="67"/>
-      <c r="G19" s="67" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="G19" s="67"/>
       <c r="H19" s="68"/>
       <c r="I19" s="68"/>
       <c r="J19" s="68"/>
@@ -2589,18 +2730,17 @@
       <c r="AA19" s="21"/>
     </row>
     <row r="20" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="24"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="34"/>
+        <v>67</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>35</v>
+      </c>
       <c r="D20" s="53"/>
       <c r="E20" s="53"/>
       <c r="F20" s="67"/>
-      <c r="G20" s="67" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="G20" s="67"/>
       <c r="H20" s="68"/>
       <c r="I20" s="68"/>
       <c r="J20" s="68"/>
@@ -2613,7 +2753,7 @@
       <c r="Q20" s="68"/>
       <c r="R20" s="68"/>
       <c r="S20" s="68"/>
-      <c r="T20" s="69"/>
+      <c r="T20" s="68"/>
       <c r="U20" s="21"/>
       <c r="V20" s="21"/>
       <c r="W20" s="21"/>
@@ -2623,11 +2763,13 @@
       <c r="AA20" s="21"/>
     </row>
     <row r="21" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="24"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="34"/>
+        <v>43</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>56</v>
+      </c>
       <c r="D21" s="53"/>
       <c r="E21" s="53"/>
       <c r="F21" s="67"/>
@@ -2657,15 +2799,15 @@
       <c r="AA21" s="21"/>
     </row>
     <row r="22" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="55"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
       <c r="F22" s="67"/>
       <c r="G22" s="67" t="str">
         <f t="shared" si="3"/>
@@ -2694,12 +2836,14 @@
     </row>
     <row r="23" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="24"/>
-      <c r="B23" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
+      <c r="B23" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
       <c r="F23" s="67"/>
       <c r="G23" s="67" t="str">
         <f t="shared" si="3"/>
@@ -2728,12 +2872,14 @@
     </row>
     <row r="24" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="24"/>
-      <c r="B24" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
+      <c r="B24" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
       <c r="F24" s="67"/>
       <c r="G24" s="67" t="str">
         <f t="shared" si="3"/>
@@ -2751,7 +2897,7 @@
       <c r="Q24" s="68"/>
       <c r="R24" s="68"/>
       <c r="S24" s="68"/>
-      <c r="T24" s="68"/>
+      <c r="T24" s="69"/>
       <c r="U24" s="21"/>
       <c r="V24" s="21"/>
       <c r="W24" s="21"/>
@@ -2762,17 +2908,16 @@
     </row>
     <row r="25" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="24"/>
-      <c r="B25" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
+      <c r="B25" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
       <c r="F25" s="67"/>
-      <c r="G25" s="67" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="G25" s="67"/>
       <c r="H25" s="68"/>
       <c r="I25" s="68"/>
       <c r="J25" s="68"/>
@@ -2785,7 +2930,7 @@
       <c r="Q25" s="68"/>
       <c r="R25" s="68"/>
       <c r="S25" s="68"/>
-      <c r="T25" s="68"/>
+      <c r="T25" s="69"/>
       <c r="U25" s="21"/>
       <c r="V25" s="21"/>
       <c r="W25" s="21"/>
@@ -2796,12 +2941,14 @@
     </row>
     <row r="26" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="24"/>
-      <c r="B26" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
+      <c r="B26" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
       <c r="F26" s="67"/>
       <c r="G26" s="67" t="str">
         <f t="shared" si="3"/>
@@ -2829,13 +2976,15 @@
       <c r="AA26" s="21"/>
     </row>
     <row r="27" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="24"/>
-      <c r="B27" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
+      <c r="A27" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="55"/>
       <c r="F27" s="67"/>
       <c r="G27" s="67" t="str">
         <f t="shared" si="3"/>
@@ -2863,15 +3012,15 @@
       <c r="AA27" s="21"/>
     </row>
     <row r="28" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="58"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
       <c r="F28" s="67"/>
       <c r="G28" s="67" t="str">
         <f t="shared" si="3"/>
@@ -2900,30 +3049,32 @@
     </row>
     <row r="29" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="24"/>
-      <c r="B29" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13" t="str">
+      <c r="B29" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="21"/>
-      <c r="S29" s="21"/>
-      <c r="T29" s="21"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="68"/>
+      <c r="M29" s="68"/>
+      <c r="N29" s="68"/>
+      <c r="O29" s="68"/>
+      <c r="P29" s="68"/>
+      <c r="Q29" s="68"/>
+      <c r="R29" s="68"/>
+      <c r="S29" s="68"/>
+      <c r="T29" s="68"/>
       <c r="U29" s="21"/>
       <c r="V29" s="21"/>
       <c r="W29" s="21"/>
@@ -2934,30 +3085,32 @@
     </row>
     <row r="30" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="24"/>
-      <c r="B30" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13" t="str">
+      <c r="B30" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="21"/>
-      <c r="Q30" s="21"/>
-      <c r="R30" s="21"/>
-      <c r="S30" s="21"/>
-      <c r="T30" s="21"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="68"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="68"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="68"/>
+      <c r="N30" s="68"/>
+      <c r="O30" s="68"/>
+      <c r="P30" s="68"/>
+      <c r="Q30" s="68"/>
+      <c r="R30" s="68"/>
+      <c r="S30" s="68"/>
+      <c r="T30" s="68"/>
       <c r="U30" s="21"/>
       <c r="V30" s="21"/>
       <c r="W30" s="21"/>
@@ -2968,30 +3121,32 @@
     </row>
     <row r="31" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="24"/>
-      <c r="B31" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13" t="str">
+      <c r="B31" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="21"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="68"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="68"/>
+      <c r="O31" s="68"/>
+      <c r="P31" s="68"/>
+      <c r="Q31" s="68"/>
+      <c r="R31" s="68"/>
+      <c r="S31" s="68"/>
+      <c r="T31" s="68"/>
       <c r="U31" s="21"/>
       <c r="V31" s="21"/>
       <c r="W31" s="21"/>
@@ -3002,30 +3157,28 @@
     </row>
     <row r="32" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="24"/>
-      <c r="B32" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="38"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13" t="str">
+      <c r="B32" s="42"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="21"/>
-      <c r="S32" s="21"/>
-      <c r="T32" s="21"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="68"/>
+      <c r="N32" s="68"/>
+      <c r="O32" s="68"/>
+      <c r="P32" s="68"/>
+      <c r="Q32" s="68"/>
+      <c r="R32" s="68"/>
+      <c r="S32" s="68"/>
+      <c r="T32" s="68"/>
       <c r="U32" s="21"/>
       <c r="V32" s="21"/>
       <c r="W32" s="21"/>
@@ -3035,31 +3188,33 @@
       <c r="AA32" s="21"/>
     </row>
     <row r="33" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="24"/>
-      <c r="B33" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="38"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13" t="str">
+      <c r="A33" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="37"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="21"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="68"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="68"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="68"/>
+      <c r="N33" s="68"/>
+      <c r="O33" s="68"/>
+      <c r="P33" s="68"/>
+      <c r="Q33" s="68"/>
+      <c r="R33" s="68"/>
+      <c r="S33" s="68"/>
+      <c r="T33" s="68"/>
       <c r="U33" s="21"/>
       <c r="V33" s="21"/>
       <c r="W33" s="21"/>
@@ -3069,13 +3224,15 @@
       <c r="AA33" s="21"/>
     </row>
     <row r="34" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13" t="str">
         <f t="shared" si="3"/>
@@ -3103,50 +3260,363 @@
       <c r="AA34" s="21"/>
     </row>
     <row r="35" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20" t="str">
+      <c r="A35" s="24"/>
+      <c r="B35" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="22"/>
-      <c r="R35" s="22"/>
-      <c r="S35" s="22"/>
-      <c r="T35" s="22"/>
-      <c r="U35" s="22"/>
-      <c r="V35" s="22"/>
-      <c r="W35" s="22"/>
-      <c r="X35" s="22"/>
-      <c r="Y35" s="22"/>
-      <c r="Z35" s="22"/>
-      <c r="AA35" s="22"/>
-    </row>
-    <row r="36" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F36" s="6"/>
-    </row>
-    <row r="37" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="11"/>
-      <c r="E37" s="26"/>
-    </row>
-    <row r="38" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="12"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
+      <c r="Q35" s="21"/>
+      <c r="R35" s="21"/>
+      <c r="S35" s="21"/>
+      <c r="T35" s="21"/>
+      <c r="U35" s="21"/>
+      <c r="V35" s="21"/>
+      <c r="W35" s="21"/>
+      <c r="X35" s="21"/>
+      <c r="Y35" s="21"/>
+      <c r="Z35" s="21"/>
+      <c r="AA35" s="21"/>
+    </row>
+    <row r="36" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="24"/>
+      <c r="B36" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="21"/>
+      <c r="R36" s="21"/>
+      <c r="S36" s="21"/>
+      <c r="T36" s="21"/>
+      <c r="U36" s="21"/>
+      <c r="V36" s="21"/>
+      <c r="W36" s="21"/>
+      <c r="X36" s="21"/>
+      <c r="Y36" s="21"/>
+      <c r="Z36" s="21"/>
+      <c r="AA36" s="21"/>
+    </row>
+    <row r="37" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="24"/>
+      <c r="B37" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="21"/>
+      <c r="U37" s="21"/>
+      <c r="V37" s="21"/>
+      <c r="W37" s="21"/>
+      <c r="X37" s="21"/>
+      <c r="Y37" s="21"/>
+      <c r="Z37" s="21"/>
+      <c r="AA37" s="21"/>
+    </row>
+    <row r="38" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="24"/>
+      <c r="B38" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="21"/>
+      <c r="U38" s="21"/>
+      <c r="V38" s="21"/>
+      <c r="W38" s="21"/>
+      <c r="X38" s="21"/>
+      <c r="Y38" s="21"/>
+      <c r="Z38" s="21"/>
+      <c r="AA38" s="21"/>
+    </row>
+    <row r="39" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="80"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H39" s="68"/>
+      <c r="I39" s="68"/>
+      <c r="J39" s="68"/>
+      <c r="K39" s="68"/>
+      <c r="L39" s="68"/>
+      <c r="M39" s="68"/>
+      <c r="N39" s="68"/>
+      <c r="O39" s="68"/>
+      <c r="P39" s="68"/>
+      <c r="Q39" s="68"/>
+      <c r="R39" s="68"/>
+      <c r="S39" s="68"/>
+      <c r="T39" s="68"/>
+      <c r="U39" s="21"/>
+      <c r="V39" s="21"/>
+      <c r="W39" s="21"/>
+      <c r="X39" s="21"/>
+      <c r="Y39" s="21"/>
+      <c r="Z39" s="21"/>
+      <c r="AA39" s="21"/>
+    </row>
+    <row r="40" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="24"/>
+      <c r="B40" s="83" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="84" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="85"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="21"/>
+      <c r="U40" s="21"/>
+      <c r="V40" s="21"/>
+      <c r="W40" s="21"/>
+      <c r="X40" s="21"/>
+      <c r="Y40" s="21"/>
+      <c r="Z40" s="21"/>
+      <c r="AA40" s="21"/>
+    </row>
+    <row r="41" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="24"/>
+      <c r="B41" s="83" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="84" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="85"/>
+      <c r="E41" s="85"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="21"/>
+      <c r="V41" s="21"/>
+      <c r="W41" s="21"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="21"/>
+      <c r="Z41" s="21"/>
+      <c r="AA41" s="21"/>
+    </row>
+    <row r="42" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="24"/>
+      <c r="B42" s="83" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="85"/>
+      <c r="E42" s="85"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="21"/>
+      <c r="R42" s="21"/>
+      <c r="S42" s="21"/>
+      <c r="T42" s="21"/>
+      <c r="U42" s="21"/>
+      <c r="V42" s="21"/>
+      <c r="W42" s="21"/>
+      <c r="X42" s="21"/>
+      <c r="Y42" s="21"/>
+      <c r="Z42" s="21"/>
+      <c r="AA42" s="21"/>
+    </row>
+    <row r="43" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="44"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="21"/>
+      <c r="Q43" s="21"/>
+      <c r="R43" s="21"/>
+      <c r="S43" s="21"/>
+      <c r="T43" s="21"/>
+      <c r="U43" s="21"/>
+      <c r="V43" s="21"/>
+      <c r="W43" s="21"/>
+      <c r="X43" s="21"/>
+      <c r="Y43" s="21"/>
+      <c r="Z43" s="21"/>
+      <c r="AA43" s="21"/>
+    </row>
+    <row r="44" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="19"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="22"/>
+      <c r="O44" s="22"/>
+      <c r="P44" s="22"/>
+      <c r="Q44" s="22"/>
+      <c r="R44" s="22"/>
+      <c r="S44" s="22"/>
+      <c r="T44" s="22"/>
+      <c r="U44" s="22"/>
+      <c r="V44" s="22"/>
+      <c r="W44" s="22"/>
+      <c r="X44" s="22"/>
+      <c r="Y44" s="22"/>
+      <c r="Z44" s="22"/>
+      <c r="AA44" s="22"/>
+    </row>
+    <row r="45" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="11"/>
+      <c r="E46" s="26"/>
+    </row>
+    <row r="47" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3156,22 +3626,22 @@
     <mergeCell ref="R4:V4"/>
     <mergeCell ref="W4:AA4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:K7 M5:P7 R5:U7 W5:Z7 H34:K35 M34:P35 R34:U35 W34:Z35">
+  <conditionalFormatting sqref="H5:K7 M5:P7 R5:U7 W5:Z7 H43:K44 M43:P44 R43:U44 W43:Z44">
     <cfRule type="expression" dxfId="6" priority="35">
       <formula>AND(TODAY()&gt;=H$5,TODAY()&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:K7 M7:P7 R7:U7 W7:Z7 H34:K35 M34:P35 R34:U35 W34:Z35">
+  <conditionalFormatting sqref="H7:K7 M7:P7 R7:U7 W7:Z7 H43:K44 M43:P44 R43:U44 W43:Z44">
     <cfRule type="expression" dxfId="5" priority="30" stopIfTrue="1">
       <formula>AND(task_end&gt;=H$5,task_start&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:AA7 H34:AA35">
+  <conditionalFormatting sqref="H7:AA7 H43:AA44">
     <cfRule type="expression" dxfId="4" priority="29">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7 Q7 AA7 L34:L35 Q34:Q35 V34:V35 AA34:AA35 V7">
+  <conditionalFormatting sqref="L7 Q7 AA7 L43:L44 Q43:Q44 V43:V44 AA43:AA44 V7">
     <cfRule type="expression" dxfId="3" priority="44" stopIfTrue="1">
       <formula>AND(task_end&gt;=L$5,task_start&lt;#REF!)</formula>
     </cfRule>
@@ -3181,7 +3651,7 @@
       <formula>AND(TODAY()&gt;=V$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA5 L5:L7 Q5:Q7 AA7 L34:L35 Q34:Q35 V34:V35 AA34:AA35">
+  <conditionalFormatting sqref="AA5 L5:L7 Q5:Q7 AA7 L43:L44 Q43:Q44 V43:V44 AA43:AA44">
     <cfRule type="expression" dxfId="1" priority="38">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
@@ -3207,21 +3677,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100CE8683845CA09544BDD5D2CFA119F453" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="25e64108eeebe26551eee07707bcd7de">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="490ce474-600e-4e79-85eb-56e37e2f143b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="23adf563ecffdbcf6d9713f65d527ff9" ns2:_="">
     <xsd:import namespace="490ce474-600e-4e79-85eb-56e37e2f143b"/>
@@ -3365,24 +3820,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3471B813-2B12-46F0-BD03-DECCBFECE95B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3398,4 +3851,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
-Documentación: Añadir nombre del 'Equipo A' y del reto 'ChatBOC' a la documentación.
</commit_message>
<xml_diff>
--- a/documentación/Plantilla Diagrama de Gantt.xlsx
+++ b/documentación/Plantilla Diagrama de Gantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A1B0E3-4CAC-4CB7-AC92-EB335AEFA0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222422F2-AC2F-482A-865D-B882646781E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -48,13 +48,7 @@
 Desplácese hacia abajo por la columna A para escuchar más instrucciones.</t>
   </si>
   <si>
-    <t>NOMBRE DEL RETO</t>
-  </si>
-  <si>
     <t>Escriba el nombre de la compañía en la celda B2.</t>
-  </si>
-  <si>
-    <t>Número del equipo:</t>
   </si>
   <si>
     <t>Escriba el nombre del responsable del proyecto en la celda B3. Escriba la fecha de comienzo del proyecto en la celda E3. Inicio del proyecto: la etiqueta se encuentra en la celda C3.</t>
@@ -312,6 +306,12 @@
   </si>
   <si>
     <t>Clase BDChroma</t>
+  </si>
+  <si>
+    <t>Nombre del equipo: "Equipo A".</t>
+  </si>
+  <si>
+    <t>ChatBOC</t>
   </si>
 </sst>
 </file>
@@ -1305,15 +1305,33 @@
     <xf numFmtId="166" fontId="9" fillId="49" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1325,24 +1343,6 @@
     </xf>
     <xf numFmtId="169" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2001,103 +2001,103 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="36.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="3.109375" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="3.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" hidden="1" customWidth="1"/>
     <col min="8" max="27" width="4" style="5" customWidth="1"/>
-    <col min="32" max="33" width="10.33203125"/>
+    <col min="32" max="33" width="10.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="4"/>
       <c r="E1" s="21"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="73"/>
-    </row>
-    <row r="2" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="72"/>
+    </row>
+    <row r="2" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="73"/>
+    </row>
+    <row r="3" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="74"/>
-    </row>
-    <row r="3" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
-        <v>4</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="80">
+        <v>45432</v>
+      </c>
+      <c r="E3" s="80"/>
+    </row>
+    <row r="4" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="61" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="72">
-        <v>45432</v>
-      </c>
-      <c r="E3" s="72"/>
-    </row>
-    <row r="4" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="61" t="s">
-        <v>7</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="H4" s="75">
+      <c r="H4" s="81">
         <f>H5</f>
         <v>45432</v>
       </c>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="76"/>
-      <c r="M4" s="75">
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="81">
         <f>H5+7</f>
         <v>45439</v>
       </c>
-      <c r="N4" s="76"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
-      <c r="R4" s="77">
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="83">
         <f>H5+14</f>
         <v>45446</v>
       </c>
-      <c r="S4" s="78"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="77">
+      <c r="S4" s="84"/>
+      <c r="T4" s="84"/>
+      <c r="U4" s="84"/>
+      <c r="V4" s="84"/>
+      <c r="W4" s="83">
         <f>H5+21</f>
         <v>45453</v>
       </c>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="78"/>
-      <c r="AA4" s="78"/>
-    </row>
-    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X4" s="84"/>
+      <c r="Y4" s="84"/>
+      <c r="Z4" s="84"/>
+      <c r="AA4" s="84"/>
+    </row>
+    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
@@ -2185,25 +2185,25 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H6" s="10" t="str">
         <f t="shared" ref="H6" si="1">LEFT(TEXT(H5,"ddd"),1)</f>
@@ -2214,10 +2214,10 @@
         <v>m</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K6" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f>LEFT(TEXT(K5,"ddd"),1)</f>
         <v>j</v>
       </c>
       <c r="L6" s="10" t="str">
@@ -2225,54 +2225,54 @@
         <v>v</v>
       </c>
       <c r="M6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="Q6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="R6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="T6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="U6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="W6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="X6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA6" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
         <v>18</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="S6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="T6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="U6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="V6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="W6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="X6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA6" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22" t="s">
-        <v>20</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7"/>
@@ -2280,69 +2280,69 @@
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="79"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="79"/>
-      <c r="Q7" s="79"/>
-      <c r="R7" s="79"/>
-      <c r="S7" s="79"/>
-      <c r="T7" s="79"/>
-      <c r="U7" s="79"/>
-      <c r="V7" s="79"/>
-      <c r="W7" s="79"/>
-      <c r="X7" s="79"/>
-      <c r="Y7" s="79"/>
-      <c r="Z7" s="79"/>
-      <c r="AA7" s="79"/>
-    </row>
-    <row r="8" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="74"/>
+      <c r="X7" s="74"/>
+      <c r="Y7" s="74"/>
+      <c r="Z7" s="74"/>
+      <c r="AA7" s="74"/>
+    </row>
+    <row r="8" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="44"/>
       <c r="E8" s="45"/>
       <c r="F8" s="63"/>
       <c r="G8" s="63"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="80"/>
-      <c r="L8" s="80"/>
-      <c r="M8" s="80"/>
-      <c r="N8" s="80"/>
-      <c r="O8" s="80"/>
-      <c r="P8" s="80"/>
-      <c r="Q8" s="80"/>
-      <c r="R8" s="80"/>
-      <c r="S8" s="80"/>
-      <c r="T8" s="80"/>
-      <c r="U8" s="79"/>
-      <c r="V8" s="79"/>
-      <c r="W8" s="79"/>
-      <c r="X8" s="79"/>
-      <c r="Y8" s="79"/>
-      <c r="Z8" s="79"/>
-      <c r="AA8" s="79"/>
-    </row>
-    <row r="9" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="75"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="75"/>
+      <c r="O8" s="75"/>
+      <c r="P8" s="75"/>
+      <c r="Q8" s="75"/>
+      <c r="R8" s="75"/>
+      <c r="S8" s="75"/>
+      <c r="T8" s="75"/>
+      <c r="U8" s="74"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="74"/>
+      <c r="X8" s="74"/>
+      <c r="Y8" s="74"/>
+      <c r="Z8" s="74"/>
+      <c r="AA8" s="74"/>
+    </row>
+    <row r="9" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="46">
         <f>Inicio_del_proyecto</f>
@@ -2353,40 +2353,40 @@
       </c>
       <c r="F9" s="64"/>
       <c r="G9" s="64"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="81" t="s">
-        <v>77</v>
-      </c>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="80"/>
-      <c r="N9" s="80"/>
-      <c r="O9" s="80"/>
-      <c r="P9" s="80"/>
-      <c r="Q9" s="80"/>
-      <c r="R9" s="80"/>
-      <c r="S9" s="80"/>
-      <c r="T9" s="80"/>
-      <c r="U9" s="79"/>
-      <c r="V9" s="79"/>
-      <c r="W9" s="79"/>
-      <c r="X9" s="79" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y9" s="79"/>
-      <c r="Z9" s="79"/>
-      <c r="AA9" s="79"/>
-    </row>
-    <row r="10" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="74"/>
+      <c r="V9" s="74"/>
+      <c r="W9" s="74"/>
+      <c r="X9" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y9" s="74"/>
+      <c r="Z9" s="74"/>
+      <c r="AA9" s="74"/>
+    </row>
+    <row r="10" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D10" s="46">
         <f>Inicio_del_proyecto</f>
@@ -2397,36 +2397,36 @@
       </c>
       <c r="F10" s="63"/>
       <c r="G10" s="63"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81" t="s">
-        <v>77</v>
-      </c>
-      <c r="K10" s="80"/>
-      <c r="L10" s="80"/>
-      <c r="M10" s="80"/>
-      <c r="N10" s="80"/>
-      <c r="O10" s="80"/>
-      <c r="P10" s="80"/>
-      <c r="Q10" s="80"/>
-      <c r="R10" s="80"/>
-      <c r="S10" s="80"/>
-      <c r="T10" s="80"/>
-      <c r="U10" s="79"/>
-      <c r="V10" s="79"/>
-      <c r="W10" s="79"/>
-      <c r="X10" s="79"/>
-      <c r="Y10" s="79"/>
-      <c r="Z10" s="79"/>
-      <c r="AA10" s="79"/>
-    </row>
-    <row r="11" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="75"/>
+      <c r="O10" s="75"/>
+      <c r="P10" s="75"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="75"/>
+      <c r="S10" s="75"/>
+      <c r="T10" s="75"/>
+      <c r="U10" s="74"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="74"/>
+      <c r="X10" s="74"/>
+      <c r="Y10" s="74"/>
+      <c r="Z10" s="74"/>
+      <c r="AA10" s="74"/>
+    </row>
+    <row r="11" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="38" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D11" s="46">
         <f>Inicio_del_proyecto</f>
@@ -2435,34 +2435,34 @@
       <c r="E11" s="46"/>
       <c r="F11" s="63"/>
       <c r="G11" s="63"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="80"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="80"/>
-      <c r="M11" s="80"/>
-      <c r="N11" s="80"/>
-      <c r="O11" s="80"/>
-      <c r="P11" s="80"/>
-      <c r="Q11" s="80"/>
-      <c r="R11" s="80"/>
-      <c r="S11" s="80"/>
-      <c r="T11" s="80"/>
-      <c r="U11" s="79"/>
-      <c r="V11" s="79"/>
-      <c r="W11" s="79"/>
-      <c r="X11" s="79"/>
-      <c r="Y11" s="79"/>
-      <c r="Z11" s="79"/>
-      <c r="AA11" s="79"/>
-    </row>
-    <row r="12" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="75"/>
+      <c r="N11" s="75"/>
+      <c r="O11" s="75"/>
+      <c r="P11" s="75"/>
+      <c r="Q11" s="75"/>
+      <c r="R11" s="75"/>
+      <c r="S11" s="75"/>
+      <c r="T11" s="75"/>
+      <c r="U11" s="74"/>
+      <c r="V11" s="74"/>
+      <c r="W11" s="74"/>
+      <c r="X11" s="74"/>
+      <c r="Y11" s="74"/>
+      <c r="Z11" s="74"/>
+      <c r="AA11" s="74"/>
+    </row>
+    <row r="12" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="46">
         <f>Inicio_del_proyecto</f>
@@ -2471,34 +2471,34 @@
       <c r="E12" s="46"/>
       <c r="F12" s="63"/>
       <c r="G12" s="63"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="80"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="80"/>
-      <c r="M12" s="80"/>
-      <c r="N12" s="80"/>
-      <c r="O12" s="80"/>
-      <c r="P12" s="80"/>
-      <c r="Q12" s="80"/>
-      <c r="R12" s="80"/>
-      <c r="S12" s="80"/>
-      <c r="T12" s="80"/>
-      <c r="U12" s="79"/>
-      <c r="V12" s="79"/>
-      <c r="W12" s="79"/>
-      <c r="X12" s="79"/>
-      <c r="Y12" s="79"/>
-      <c r="Z12" s="79"/>
-      <c r="AA12" s="79"/>
-    </row>
-    <row r="13" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H12" s="77"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="75"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="75"/>
+      <c r="O12" s="75"/>
+      <c r="P12" s="75"/>
+      <c r="Q12" s="75"/>
+      <c r="R12" s="75"/>
+      <c r="S12" s="75"/>
+      <c r="T12" s="75"/>
+      <c r="U12" s="74"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="74"/>
+      <c r="X12" s="74"/>
+      <c r="Y12" s="74"/>
+      <c r="Z12" s="74"/>
+      <c r="AA12" s="74"/>
+    </row>
+    <row r="13" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="46">
         <f>Inicio_del_proyecto</f>
@@ -2507,165 +2507,165 @@
       <c r="E13" s="46"/>
       <c r="F13" s="63"/>
       <c r="G13" s="63"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="80"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="80"/>
-      <c r="P13" s="80"/>
-      <c r="Q13" s="80"/>
-      <c r="R13" s="80"/>
-      <c r="S13" s="80"/>
-      <c r="T13" s="80"/>
-      <c r="U13" s="79"/>
-      <c r="V13" s="79"/>
-      <c r="W13" s="79"/>
-      <c r="X13" s="79"/>
-      <c r="Y13" s="79"/>
-      <c r="Z13" s="79"/>
-      <c r="AA13" s="79"/>
-    </row>
-    <row r="14" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="77"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="75"/>
+      <c r="N13" s="75"/>
+      <c r="O13" s="75"/>
+      <c r="P13" s="75"/>
+      <c r="Q13" s="75"/>
+      <c r="R13" s="75"/>
+      <c r="S13" s="75"/>
+      <c r="T13" s="75"/>
+      <c r="U13" s="74"/>
+      <c r="V13" s="74"/>
+      <c r="W13" s="74"/>
+      <c r="X13" s="74"/>
+      <c r="Y13" s="74"/>
+      <c r="Z13" s="74"/>
+      <c r="AA13" s="74"/>
+    </row>
+    <row r="14" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" s="38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D14" s="46"/>
       <c r="E14" s="46"/>
       <c r="F14" s="63"/>
       <c r="G14" s="63"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="80"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="80"/>
-      <c r="M14" s="80"/>
-      <c r="N14" s="80"/>
-      <c r="O14" s="80"/>
-      <c r="P14" s="80"/>
-      <c r="Q14" s="80"/>
-      <c r="R14" s="80"/>
-      <c r="S14" s="80"/>
-      <c r="T14" s="80"/>
-      <c r="U14" s="79"/>
-      <c r="V14" s="79"/>
-      <c r="W14" s="79"/>
-      <c r="X14" s="79"/>
-      <c r="Y14" s="79"/>
-      <c r="Z14" s="79"/>
-      <c r="AA14" s="79"/>
-    </row>
-    <row r="15" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H14" s="78"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="75"/>
+      <c r="M14" s="75"/>
+      <c r="N14" s="75"/>
+      <c r="O14" s="75"/>
+      <c r="P14" s="75"/>
+      <c r="Q14" s="75"/>
+      <c r="R14" s="75"/>
+      <c r="S14" s="75"/>
+      <c r="T14" s="75"/>
+      <c r="U14" s="74"/>
+      <c r="V14" s="74"/>
+      <c r="W14" s="74"/>
+      <c r="X14" s="74"/>
+      <c r="Y14" s="74"/>
+      <c r="Z14" s="74"/>
+      <c r="AA14" s="74"/>
+    </row>
+    <row r="15" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" s="38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="46"/>
       <c r="E15" s="46"/>
       <c r="F15" s="63"/>
       <c r="G15" s="63"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="80"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="80"/>
-      <c r="M15" s="80"/>
-      <c r="N15" s="80"/>
-      <c r="O15" s="80"/>
-      <c r="P15" s="80"/>
-      <c r="Q15" s="80"/>
-      <c r="R15" s="80"/>
-      <c r="S15" s="80"/>
-      <c r="T15" s="80"/>
-      <c r="U15" s="79"/>
-      <c r="V15" s="79"/>
-      <c r="W15" s="79"/>
-      <c r="X15" s="79"/>
-      <c r="Y15" s="79"/>
-      <c r="Z15" s="79"/>
-      <c r="AA15" s="79"/>
-    </row>
-    <row r="16" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H15" s="78"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="75"/>
+      <c r="L15" s="75"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="75"/>
+      <c r="O15" s="75"/>
+      <c r="P15" s="75"/>
+      <c r="Q15" s="75"/>
+      <c r="R15" s="75"/>
+      <c r="S15" s="75"/>
+      <c r="T15" s="75"/>
+      <c r="U15" s="74"/>
+      <c r="V15" s="74"/>
+      <c r="W15" s="74"/>
+      <c r="X15" s="74"/>
+      <c r="Y15" s="74"/>
+      <c r="Z15" s="74"/>
+      <c r="AA15" s="74"/>
+    </row>
+    <row r="16" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22"/>
       <c r="B16" s="38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D16" s="46"/>
       <c r="E16" s="46"/>
       <c r="F16" s="63"/>
       <c r="G16" s="63"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="80"/>
-      <c r="M16" s="80"/>
-      <c r="N16" s="80"/>
-      <c r="O16" s="80"/>
-      <c r="P16" s="80"/>
-      <c r="Q16" s="80"/>
-      <c r="R16" s="80"/>
-      <c r="S16" s="80"/>
-      <c r="T16" s="80"/>
-      <c r="U16" s="79"/>
-      <c r="V16" s="79"/>
-      <c r="W16" s="79"/>
-      <c r="X16" s="79"/>
-      <c r="Y16" s="79"/>
-      <c r="Z16" s="79"/>
-      <c r="AA16" s="79"/>
-    </row>
-    <row r="17" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H16" s="78"/>
+      <c r="I16" s="75"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="75"/>
+      <c r="L16" s="75"/>
+      <c r="M16" s="75"/>
+      <c r="N16" s="75"/>
+      <c r="O16" s="75"/>
+      <c r="P16" s="75"/>
+      <c r="Q16" s="75"/>
+      <c r="R16" s="75"/>
+      <c r="S16" s="75"/>
+      <c r="T16" s="75"/>
+      <c r="U16" s="74"/>
+      <c r="V16" s="74"/>
+      <c r="W16" s="74"/>
+      <c r="X16" s="74"/>
+      <c r="Y16" s="74"/>
+      <c r="Z16" s="74"/>
+      <c r="AA16" s="74"/>
+    </row>
+    <row r="17" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
       <c r="B17" s="38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D17" s="46"/>
       <c r="E17" s="46"/>
       <c r="F17" s="63"/>
       <c r="G17" s="63"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="80"/>
-      <c r="M17" s="80"/>
-      <c r="N17" s="80"/>
-      <c r="O17" s="80"/>
-      <c r="P17" s="80"/>
-      <c r="Q17" s="80"/>
-      <c r="R17" s="80"/>
-      <c r="S17" s="80"/>
-      <c r="T17" s="80"/>
-      <c r="U17" s="79"/>
-      <c r="V17" s="79"/>
-      <c r="W17" s="79"/>
-      <c r="X17" s="79"/>
-      <c r="Y17" s="79"/>
-      <c r="Z17" s="79"/>
-      <c r="AA17" s="79"/>
-    </row>
-    <row r="18" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H17" s="77"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="75"/>
+      <c r="L17" s="75"/>
+      <c r="M17" s="75"/>
+      <c r="N17" s="75"/>
+      <c r="O17" s="75"/>
+      <c r="P17" s="75"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="75"/>
+      <c r="S17" s="75"/>
+      <c r="T17" s="75"/>
+      <c r="U17" s="74"/>
+      <c r="V17" s="74"/>
+      <c r="W17" s="74"/>
+      <c r="X17" s="74"/>
+      <c r="Y17" s="74"/>
+      <c r="Z17" s="74"/>
+      <c r="AA17" s="74"/>
+    </row>
+    <row r="18" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="47"/>
@@ -2675,34 +2675,34 @@
         <f t="shared" ref="G18:G45" si="3">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="H18" s="80"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
-      <c r="N18" s="80"/>
-      <c r="O18" s="80"/>
-      <c r="P18" s="80"/>
-      <c r="Q18" s="80"/>
-      <c r="R18" s="80"/>
-      <c r="S18" s="80"/>
-      <c r="T18" s="80"/>
-      <c r="U18" s="79"/>
-      <c r="V18" s="79"/>
-      <c r="W18" s="79"/>
-      <c r="X18" s="79"/>
-      <c r="Y18" s="79"/>
-      <c r="Z18" s="79"/>
-      <c r="AA18" s="79"/>
-    </row>
-    <row r="19" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="75"/>
+      <c r="N18" s="75"/>
+      <c r="O18" s="75"/>
+      <c r="P18" s="75"/>
+      <c r="Q18" s="75"/>
+      <c r="R18" s="75"/>
+      <c r="S18" s="75"/>
+      <c r="T18" s="75"/>
+      <c r="U18" s="74"/>
+      <c r="V18" s="74"/>
+      <c r="W18" s="74"/>
+      <c r="X18" s="74"/>
+      <c r="Y18" s="74"/>
+      <c r="Z18" s="74"/>
+      <c r="AA18" s="74"/>
+    </row>
+    <row r="19" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23"/>
       <c r="B19" s="39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19" s="49"/>
       <c r="E19" s="49"/>
@@ -2711,100 +2711,100 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H19" s="80"/>
-      <c r="I19" s="80"/>
-      <c r="J19" s="80"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="80"/>
-      <c r="M19" s="80"/>
-      <c r="N19" s="80"/>
-      <c r="O19" s="80"/>
-      <c r="P19" s="80"/>
-      <c r="Q19" s="80"/>
-      <c r="R19" s="80"/>
-      <c r="S19" s="80"/>
-      <c r="T19" s="80"/>
-      <c r="U19" s="79"/>
-      <c r="V19" s="79"/>
-      <c r="W19" s="79"/>
-      <c r="X19" s="79"/>
-      <c r="Y19" s="79"/>
-      <c r="Z19" s="79"/>
-      <c r="AA19" s="79"/>
-    </row>
-    <row r="20" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="75"/>
+      <c r="L19" s="75"/>
+      <c r="M19" s="75"/>
+      <c r="N19" s="75"/>
+      <c r="O19" s="75"/>
+      <c r="P19" s="75"/>
+      <c r="Q19" s="75"/>
+      <c r="R19" s="75"/>
+      <c r="S19" s="75"/>
+      <c r="T19" s="75"/>
+      <c r="U19" s="74"/>
+      <c r="V19" s="74"/>
+      <c r="W19" s="74"/>
+      <c r="X19" s="74"/>
+      <c r="Y19" s="74"/>
+      <c r="Z19" s="74"/>
+      <c r="AA19" s="74"/>
+    </row>
+    <row r="20" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23"/>
       <c r="B20" s="39" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" s="49"/>
       <c r="E20" s="49"/>
       <c r="F20" s="63"/>
       <c r="G20" s="63"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="80"/>
-      <c r="K20" s="80"/>
-      <c r="L20" s="80"/>
-      <c r="M20" s="80"/>
-      <c r="N20" s="80"/>
-      <c r="O20" s="80"/>
-      <c r="P20" s="80"/>
-      <c r="Q20" s="80"/>
-      <c r="R20" s="80"/>
-      <c r="S20" s="80"/>
-      <c r="T20" s="80"/>
-      <c r="U20" s="79"/>
-      <c r="V20" s="79"/>
-      <c r="W20" s="79"/>
-      <c r="X20" s="79"/>
-      <c r="Y20" s="79"/>
-      <c r="Z20" s="79"/>
-      <c r="AA20" s="79"/>
-    </row>
-    <row r="21" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="75"/>
+      <c r="N20" s="75"/>
+      <c r="O20" s="75"/>
+      <c r="P20" s="75"/>
+      <c r="Q20" s="75"/>
+      <c r="R20" s="75"/>
+      <c r="S20" s="75"/>
+      <c r="T20" s="75"/>
+      <c r="U20" s="74"/>
+      <c r="V20" s="74"/>
+      <c r="W20" s="74"/>
+      <c r="X20" s="74"/>
+      <c r="Y20" s="74"/>
+      <c r="Z20" s="74"/>
+      <c r="AA20" s="74"/>
+    </row>
+    <row r="21" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="23"/>
       <c r="B21" s="39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D21" s="49"/>
       <c r="E21" s="49"/>
       <c r="F21" s="63"/>
       <c r="G21" s="63"/>
-      <c r="H21" s="80"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="80"/>
-      <c r="K21" s="80"/>
-      <c r="L21" s="80"/>
-      <c r="M21" s="80"/>
-      <c r="N21" s="80"/>
-      <c r="O21" s="80"/>
-      <c r="P21" s="80"/>
-      <c r="Q21" s="80"/>
-      <c r="R21" s="80"/>
-      <c r="S21" s="80"/>
-      <c r="T21" s="80"/>
-      <c r="U21" s="79"/>
-      <c r="V21" s="79"/>
-      <c r="W21" s="79"/>
-      <c r="X21" s="79"/>
-      <c r="Y21" s="79"/>
-      <c r="Z21" s="79"/>
-      <c r="AA21" s="79"/>
-    </row>
-    <row r="22" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H21" s="75"/>
+      <c r="I21" s="75"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="75"/>
+      <c r="L21" s="75"/>
+      <c r="M21" s="75"/>
+      <c r="N21" s="75"/>
+      <c r="O21" s="75"/>
+      <c r="P21" s="75"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="75"/>
+      <c r="S21" s="75"/>
+      <c r="T21" s="75"/>
+      <c r="U21" s="74"/>
+      <c r="V21" s="74"/>
+      <c r="W21" s="74"/>
+      <c r="X21" s="74"/>
+      <c r="Y21" s="74"/>
+      <c r="Z21" s="74"/>
+      <c r="AA21" s="74"/>
+    </row>
+    <row r="22" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="23"/>
       <c r="B22" s="39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="49"/>
@@ -2813,34 +2813,34 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H22" s="80"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="80"/>
-      <c r="L22" s="80"/>
-      <c r="M22" s="80"/>
-      <c r="N22" s="80"/>
-      <c r="O22" s="80"/>
-      <c r="P22" s="80"/>
-      <c r="Q22" s="80"/>
-      <c r="R22" s="80"/>
-      <c r="S22" s="80"/>
-      <c r="T22" s="80"/>
-      <c r="U22" s="79"/>
-      <c r="V22" s="79"/>
-      <c r="W22" s="79"/>
-      <c r="X22" s="79"/>
-      <c r="Y22" s="79"/>
-      <c r="Z22" s="79"/>
-      <c r="AA22" s="79"/>
-    </row>
-    <row r="23" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H22" s="75"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="75"/>
+      <c r="K22" s="75"/>
+      <c r="L22" s="75"/>
+      <c r="M22" s="75"/>
+      <c r="N22" s="75"/>
+      <c r="O22" s="75"/>
+      <c r="P22" s="75"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="75"/>
+      <c r="S22" s="75"/>
+      <c r="T22" s="75"/>
+      <c r="U22" s="74"/>
+      <c r="V22" s="74"/>
+      <c r="W22" s="74"/>
+      <c r="X22" s="74"/>
+      <c r="Y22" s="74"/>
+      <c r="Z22" s="74"/>
+      <c r="AA22" s="74"/>
+    </row>
+    <row r="23" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D23" s="49"/>
       <c r="E23" s="49"/>
@@ -2849,34 +2849,34 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H23" s="80"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="80"/>
-      <c r="K23" s="80"/>
-      <c r="L23" s="80"/>
-      <c r="M23" s="80"/>
-      <c r="N23" s="80"/>
-      <c r="O23" s="80"/>
-      <c r="P23" s="80"/>
-      <c r="Q23" s="80"/>
-      <c r="R23" s="80"/>
-      <c r="S23" s="80"/>
-      <c r="T23" s="80"/>
-      <c r="U23" s="79"/>
-      <c r="V23" s="79"/>
-      <c r="W23" s="79"/>
-      <c r="X23" s="79"/>
-      <c r="Y23" s="79"/>
-      <c r="Z23" s="79"/>
-      <c r="AA23" s="79"/>
-    </row>
-    <row r="24" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
+      <c r="M23" s="75"/>
+      <c r="N23" s="75"/>
+      <c r="O23" s="75"/>
+      <c r="P23" s="75"/>
+      <c r="Q23" s="75"/>
+      <c r="R23" s="75"/>
+      <c r="S23" s="75"/>
+      <c r="T23" s="75"/>
+      <c r="U23" s="74"/>
+      <c r="V23" s="74"/>
+      <c r="W23" s="74"/>
+      <c r="X23" s="74"/>
+      <c r="Y23" s="74"/>
+      <c r="Z23" s="74"/>
+      <c r="AA23" s="74"/>
+    </row>
+    <row r="24" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="39" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D24" s="49"/>
       <c r="E24" s="49"/>
@@ -2885,34 +2885,34 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="80"/>
-      <c r="L24" s="80"/>
-      <c r="M24" s="80"/>
-      <c r="N24" s="80"/>
-      <c r="O24" s="80"/>
-      <c r="P24" s="80"/>
-      <c r="Q24" s="80"/>
-      <c r="R24" s="80"/>
-      <c r="S24" s="80"/>
-      <c r="T24" s="80"/>
-      <c r="U24" s="79"/>
-      <c r="V24" s="79"/>
-      <c r="W24" s="79"/>
-      <c r="X24" s="79"/>
-      <c r="Y24" s="79"/>
-      <c r="Z24" s="79"/>
-      <c r="AA24" s="79"/>
-    </row>
-    <row r="25" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="75"/>
+      <c r="O24" s="75"/>
+      <c r="P24" s="75"/>
+      <c r="Q24" s="75"/>
+      <c r="R24" s="75"/>
+      <c r="S24" s="75"/>
+      <c r="T24" s="75"/>
+      <c r="U24" s="74"/>
+      <c r="V24" s="74"/>
+      <c r="W24" s="74"/>
+      <c r="X24" s="74"/>
+      <c r="Y24" s="74"/>
+      <c r="Z24" s="74"/>
+      <c r="AA24" s="74"/>
+    </row>
+    <row r="25" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D25" s="49"/>
       <c r="E25" s="49"/>
@@ -2921,67 +2921,67 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="80"/>
-      <c r="M25" s="80"/>
-      <c r="N25" s="80"/>
-      <c r="O25" s="80"/>
-      <c r="P25" s="80"/>
-      <c r="Q25" s="80"/>
-      <c r="R25" s="80"/>
-      <c r="S25" s="80"/>
-      <c r="T25" s="80"/>
-      <c r="U25" s="79"/>
-      <c r="V25" s="79"/>
-      <c r="W25" s="79"/>
-      <c r="X25" s="79"/>
-      <c r="Y25" s="79"/>
-      <c r="Z25" s="79"/>
-      <c r="AA25" s="79"/>
-    </row>
-    <row r="26" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="75"/>
+      <c r="L25" s="75"/>
+      <c r="M25" s="75"/>
+      <c r="N25" s="75"/>
+      <c r="O25" s="75"/>
+      <c r="P25" s="75"/>
+      <c r="Q25" s="75"/>
+      <c r="R25" s="75"/>
+      <c r="S25" s="75"/>
+      <c r="T25" s="75"/>
+      <c r="U25" s="74"/>
+      <c r="V25" s="74"/>
+      <c r="W25" s="74"/>
+      <c r="X25" s="74"/>
+      <c r="Y25" s="74"/>
+      <c r="Z25" s="74"/>
+      <c r="AA25" s="74"/>
+    </row>
+    <row r="26" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D26" s="49"/>
       <c r="E26" s="49"/>
       <c r="F26" s="63"/>
       <c r="G26" s="63"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="80"/>
-      <c r="L26" s="80"/>
-      <c r="M26" s="80"/>
-      <c r="N26" s="80"/>
-      <c r="O26" s="80"/>
-      <c r="P26" s="80"/>
-      <c r="Q26" s="80"/>
-      <c r="R26" s="80"/>
-      <c r="S26" s="80"/>
-      <c r="T26" s="80"/>
-      <c r="U26" s="79"/>
-      <c r="V26" s="79"/>
-      <c r="W26" s="79"/>
-      <c r="X26" s="79"/>
-      <c r="Y26" s="79"/>
-      <c r="Z26" s="79"/>
-      <c r="AA26" s="79"/>
-    </row>
-    <row r="27" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="75"/>
+      <c r="M26" s="75"/>
+      <c r="N26" s="75"/>
+      <c r="O26" s="75"/>
+      <c r="P26" s="75"/>
+      <c r="Q26" s="75"/>
+      <c r="R26" s="75"/>
+      <c r="S26" s="75"/>
+      <c r="T26" s="75"/>
+      <c r="U26" s="74"/>
+      <c r="V26" s="74"/>
+      <c r="W26" s="74"/>
+      <c r="X26" s="74"/>
+      <c r="Y26" s="74"/>
+      <c r="Z26" s="74"/>
+      <c r="AA26" s="74"/>
+    </row>
+    <row r="27" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="22"/>
       <c r="B27" s="39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D27" s="49"/>
       <c r="E27" s="49"/>
@@ -2990,33 +2990,33 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H27" s="80"/>
-      <c r="I27" s="80"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="80"/>
-      <c r="L27" s="80"/>
-      <c r="M27" s="80"/>
-      <c r="N27" s="80"/>
-      <c r="O27" s="80"/>
-      <c r="P27" s="80"/>
-      <c r="Q27" s="80"/>
-      <c r="R27" s="80"/>
-      <c r="S27" s="80"/>
-      <c r="T27" s="80"/>
-      <c r="U27" s="79"/>
-      <c r="V27" s="79"/>
-      <c r="W27" s="79"/>
-      <c r="X27" s="79"/>
-      <c r="Y27" s="79"/>
-      <c r="Z27" s="79"/>
-      <c r="AA27" s="79"/>
-    </row>
-    <row r="28" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="75"/>
+      <c r="M27" s="75"/>
+      <c r="N27" s="75"/>
+      <c r="O27" s="75"/>
+      <c r="P27" s="75"/>
+      <c r="Q27" s="75"/>
+      <c r="R27" s="75"/>
+      <c r="S27" s="75"/>
+      <c r="T27" s="75"/>
+      <c r="U27" s="74"/>
+      <c r="V27" s="74"/>
+      <c r="W27" s="74"/>
+      <c r="X27" s="74"/>
+      <c r="Y27" s="74"/>
+      <c r="Z27" s="74"/>
+      <c r="AA27" s="74"/>
+    </row>
+    <row r="28" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="50"/>
@@ -3026,34 +3026,34 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H28" s="80"/>
-      <c r="I28" s="80"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="80"/>
-      <c r="L28" s="80"/>
-      <c r="M28" s="80"/>
-      <c r="N28" s="80"/>
-      <c r="O28" s="80"/>
-      <c r="P28" s="80"/>
-      <c r="Q28" s="80"/>
-      <c r="R28" s="80"/>
-      <c r="S28" s="80"/>
-      <c r="T28" s="80"/>
-      <c r="U28" s="79"/>
-      <c r="V28" s="79"/>
-      <c r="W28" s="79"/>
-      <c r="X28" s="79"/>
-      <c r="Y28" s="79"/>
-      <c r="Z28" s="79"/>
-      <c r="AA28" s="79"/>
-    </row>
-    <row r="29" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
+      <c r="J28" s="75"/>
+      <c r="K28" s="75"/>
+      <c r="L28" s="75"/>
+      <c r="M28" s="75"/>
+      <c r="N28" s="75"/>
+      <c r="O28" s="75"/>
+      <c r="P28" s="75"/>
+      <c r="Q28" s="75"/>
+      <c r="R28" s="75"/>
+      <c r="S28" s="75"/>
+      <c r="T28" s="75"/>
+      <c r="U28" s="74"/>
+      <c r="V28" s="74"/>
+      <c r="W28" s="74"/>
+      <c r="X28" s="74"/>
+      <c r="Y28" s="74"/>
+      <c r="Z28" s="74"/>
+      <c r="AA28" s="74"/>
+    </row>
+    <row r="29" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22"/>
       <c r="B29" s="40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D29" s="52"/>
       <c r="E29" s="52"/>
@@ -3062,34 +3062,34 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H29" s="80"/>
-      <c r="I29" s="80"/>
-      <c r="J29" s="80"/>
-      <c r="K29" s="80"/>
-      <c r="L29" s="80"/>
-      <c r="M29" s="80"/>
-      <c r="N29" s="80"/>
-      <c r="O29" s="80"/>
-      <c r="P29" s="80"/>
-      <c r="Q29" s="80"/>
-      <c r="R29" s="80"/>
-      <c r="S29" s="80"/>
-      <c r="T29" s="80"/>
-      <c r="U29" s="79"/>
-      <c r="V29" s="79"/>
-      <c r="W29" s="79"/>
-      <c r="X29" s="79"/>
-      <c r="Y29" s="79"/>
-      <c r="Z29" s="79"/>
-      <c r="AA29" s="79"/>
-    </row>
-    <row r="30" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="75"/>
+      <c r="L29" s="75"/>
+      <c r="M29" s="75"/>
+      <c r="N29" s="75"/>
+      <c r="O29" s="75"/>
+      <c r="P29" s="75"/>
+      <c r="Q29" s="75"/>
+      <c r="R29" s="75"/>
+      <c r="S29" s="75"/>
+      <c r="T29" s="75"/>
+      <c r="U29" s="74"/>
+      <c r="V29" s="74"/>
+      <c r="W29" s="74"/>
+      <c r="X29" s="74"/>
+      <c r="Y29" s="74"/>
+      <c r="Z29" s="74"/>
+      <c r="AA29" s="74"/>
+    </row>
+    <row r="30" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="22"/>
       <c r="B30" s="40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D30" s="52"/>
       <c r="E30" s="52"/>
@@ -3098,34 +3098,34 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H30" s="80"/>
-      <c r="I30" s="80"/>
-      <c r="J30" s="80"/>
-      <c r="K30" s="80"/>
-      <c r="L30" s="80"/>
-      <c r="M30" s="80"/>
-      <c r="N30" s="80"/>
-      <c r="O30" s="80"/>
-      <c r="P30" s="80"/>
-      <c r="Q30" s="80"/>
-      <c r="R30" s="80"/>
-      <c r="S30" s="80"/>
-      <c r="T30" s="80"/>
-      <c r="U30" s="79"/>
-      <c r="V30" s="79"/>
-      <c r="W30" s="79"/>
-      <c r="X30" s="79"/>
-      <c r="Y30" s="79"/>
-      <c r="Z30" s="79"/>
-      <c r="AA30" s="79"/>
-    </row>
-    <row r="31" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H30" s="75"/>
+      <c r="I30" s="75"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="75"/>
+      <c r="M30" s="75"/>
+      <c r="N30" s="75"/>
+      <c r="O30" s="75"/>
+      <c r="P30" s="75"/>
+      <c r="Q30" s="75"/>
+      <c r="R30" s="75"/>
+      <c r="S30" s="75"/>
+      <c r="T30" s="75"/>
+      <c r="U30" s="74"/>
+      <c r="V30" s="74"/>
+      <c r="W30" s="74"/>
+      <c r="X30" s="74"/>
+      <c r="Y30" s="74"/>
+      <c r="Z30" s="74"/>
+      <c r="AA30" s="74"/>
+    </row>
+    <row r="31" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22"/>
       <c r="B31" s="40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D31" s="52"/>
       <c r="E31" s="52"/>
@@ -3134,34 +3134,34 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H31" s="80"/>
-      <c r="I31" s="80"/>
-      <c r="J31" s="80"/>
-      <c r="K31" s="80"/>
-      <c r="L31" s="80"/>
-      <c r="M31" s="80"/>
-      <c r="N31" s="80"/>
-      <c r="O31" s="80"/>
-      <c r="P31" s="80"/>
-      <c r="Q31" s="80"/>
-      <c r="R31" s="80"/>
-      <c r="S31" s="80"/>
-      <c r="T31" s="80"/>
-      <c r="U31" s="79"/>
-      <c r="V31" s="79"/>
-      <c r="W31" s="79"/>
-      <c r="X31" s="79"/>
-      <c r="Y31" s="79"/>
-      <c r="Z31" s="79"/>
-      <c r="AA31" s="79"/>
-    </row>
-    <row r="32" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H31" s="75"/>
+      <c r="I31" s="75"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="75"/>
+      <c r="M31" s="75"/>
+      <c r="N31" s="75"/>
+      <c r="O31" s="75"/>
+      <c r="P31" s="75"/>
+      <c r="Q31" s="75"/>
+      <c r="R31" s="75"/>
+      <c r="S31" s="75"/>
+      <c r="T31" s="75"/>
+      <c r="U31" s="74"/>
+      <c r="V31" s="74"/>
+      <c r="W31" s="74"/>
+      <c r="X31" s="74"/>
+      <c r="Y31" s="74"/>
+      <c r="Z31" s="74"/>
+      <c r="AA31" s="74"/>
+    </row>
+    <row r="32" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22"/>
       <c r="B32" s="40" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D32" s="52"/>
       <c r="E32" s="52"/>
@@ -3170,28 +3170,28 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H32" s="80"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="80"/>
-      <c r="K32" s="80"/>
-      <c r="L32" s="80"/>
-      <c r="M32" s="80"/>
-      <c r="N32" s="80"/>
-      <c r="O32" s="80"/>
-      <c r="P32" s="80"/>
-      <c r="Q32" s="80"/>
-      <c r="R32" s="80"/>
-      <c r="S32" s="80"/>
-      <c r="T32" s="80"/>
-      <c r="U32" s="79"/>
-      <c r="V32" s="79"/>
-      <c r="W32" s="79"/>
-      <c r="X32" s="79"/>
-      <c r="Y32" s="79"/>
-      <c r="Z32" s="79"/>
-      <c r="AA32" s="79"/>
-    </row>
-    <row r="33" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H32" s="75"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="75"/>
+      <c r="M32" s="75"/>
+      <c r="N32" s="75"/>
+      <c r="O32" s="75"/>
+      <c r="P32" s="75"/>
+      <c r="Q32" s="75"/>
+      <c r="R32" s="75"/>
+      <c r="S32" s="75"/>
+      <c r="T32" s="75"/>
+      <c r="U32" s="74"/>
+      <c r="V32" s="74"/>
+      <c r="W32" s="74"/>
+      <c r="X32" s="74"/>
+      <c r="Y32" s="74"/>
+      <c r="Z32" s="74"/>
+      <c r="AA32" s="74"/>
+    </row>
+    <row r="33" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="22"/>
       <c r="B33" s="40"/>
       <c r="C33" s="34"/>
@@ -3202,33 +3202,33 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H33" s="80"/>
-      <c r="I33" s="80"/>
-      <c r="J33" s="80"/>
-      <c r="K33" s="80"/>
-      <c r="L33" s="80"/>
-      <c r="M33" s="80"/>
-      <c r="N33" s="80"/>
-      <c r="O33" s="80"/>
-      <c r="P33" s="80"/>
-      <c r="Q33" s="80"/>
-      <c r="R33" s="80"/>
-      <c r="S33" s="80"/>
-      <c r="T33" s="80"/>
-      <c r="U33" s="79"/>
-      <c r="V33" s="79"/>
-      <c r="W33" s="79"/>
-      <c r="X33" s="79"/>
-      <c r="Y33" s="79"/>
-      <c r="Z33" s="79"/>
-      <c r="AA33" s="79"/>
-    </row>
-    <row r="34" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H33" s="75"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="75"/>
+      <c r="L33" s="75"/>
+      <c r="M33" s="75"/>
+      <c r="N33" s="75"/>
+      <c r="O33" s="75"/>
+      <c r="P33" s="75"/>
+      <c r="Q33" s="75"/>
+      <c r="R33" s="75"/>
+      <c r="S33" s="75"/>
+      <c r="T33" s="75"/>
+      <c r="U33" s="74"/>
+      <c r="V33" s="74"/>
+      <c r="W33" s="74"/>
+      <c r="X33" s="74"/>
+      <c r="Y33" s="74"/>
+      <c r="Z33" s="74"/>
+      <c r="AA33" s="74"/>
+    </row>
+    <row r="34" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C34" s="35"/>
       <c r="D34" s="53"/>
@@ -3238,34 +3238,34 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H34" s="80"/>
-      <c r="I34" s="80"/>
-      <c r="J34" s="80"/>
-      <c r="K34" s="80"/>
-      <c r="L34" s="80"/>
-      <c r="M34" s="80"/>
-      <c r="N34" s="80"/>
-      <c r="O34" s="80"/>
-      <c r="P34" s="80"/>
-      <c r="Q34" s="80"/>
-      <c r="R34" s="80"/>
-      <c r="S34" s="80"/>
-      <c r="T34" s="80"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="79"/>
-      <c r="W34" s="79"/>
-      <c r="X34" s="79"/>
-      <c r="Y34" s="79"/>
-      <c r="Z34" s="79"/>
-      <c r="AA34" s="79"/>
-    </row>
-    <row r="35" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="75"/>
+      <c r="M34" s="75"/>
+      <c r="N34" s="75"/>
+      <c r="O34" s="75"/>
+      <c r="P34" s="75"/>
+      <c r="Q34" s="75"/>
+      <c r="R34" s="75"/>
+      <c r="S34" s="75"/>
+      <c r="T34" s="75"/>
+      <c r="U34" s="74"/>
+      <c r="V34" s="74"/>
+      <c r="W34" s="74"/>
+      <c r="X34" s="74"/>
+      <c r="Y34" s="74"/>
+      <c r="Z34" s="74"/>
+      <c r="AA34" s="74"/>
+    </row>
+    <row r="35" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22"/>
       <c r="B35" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="36" t="s">
         <v>70</v>
-      </c>
-      <c r="C35" s="36" t="s">
-        <v>72</v>
       </c>
       <c r="D35" s="55"/>
       <c r="E35" s="55"/>
@@ -3274,34 +3274,34 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H35" s="79"/>
-      <c r="I35" s="79"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="79"/>
-      <c r="N35" s="79"/>
-      <c r="O35" s="79"/>
-      <c r="P35" s="79"/>
-      <c r="Q35" s="79"/>
-      <c r="R35" s="79"/>
-      <c r="S35" s="79"/>
-      <c r="T35" s="79"/>
-      <c r="U35" s="79"/>
-      <c r="V35" s="79"/>
-      <c r="W35" s="79"/>
-      <c r="X35" s="79"/>
-      <c r="Y35" s="79"/>
-      <c r="Z35" s="79"/>
-      <c r="AA35" s="79"/>
-    </row>
-    <row r="36" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H35" s="74"/>
+      <c r="I35" s="74"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="74"/>
+      <c r="M35" s="74"/>
+      <c r="N35" s="74"/>
+      <c r="O35" s="74"/>
+      <c r="P35" s="74"/>
+      <c r="Q35" s="74"/>
+      <c r="R35" s="74"/>
+      <c r="S35" s="74"/>
+      <c r="T35" s="74"/>
+      <c r="U35" s="74"/>
+      <c r="V35" s="74"/>
+      <c r="W35" s="74"/>
+      <c r="X35" s="74"/>
+      <c r="Y35" s="74"/>
+      <c r="Z35" s="74"/>
+      <c r="AA35" s="74"/>
+    </row>
+    <row r="36" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="22"/>
       <c r="B36" s="41" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D36" s="55"/>
       <c r="E36" s="55"/>
@@ -3310,34 +3310,34 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H36" s="79"/>
-      <c r="I36" s="79"/>
-      <c r="J36" s="79"/>
-      <c r="K36" s="79"/>
-      <c r="L36" s="79"/>
-      <c r="M36" s="79"/>
-      <c r="N36" s="79"/>
-      <c r="O36" s="79"/>
-      <c r="P36" s="79"/>
-      <c r="Q36" s="79"/>
-      <c r="R36" s="79"/>
-      <c r="S36" s="79"/>
-      <c r="T36" s="79"/>
-      <c r="U36" s="79"/>
-      <c r="V36" s="79"/>
-      <c r="W36" s="79"/>
-      <c r="X36" s="79"/>
-      <c r="Y36" s="79"/>
-      <c r="Z36" s="79"/>
-      <c r="AA36" s="79"/>
-    </row>
-    <row r="37" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H36" s="74"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="74"/>
+      <c r="K36" s="74"/>
+      <c r="L36" s="74"/>
+      <c r="M36" s="74"/>
+      <c r="N36" s="74"/>
+      <c r="O36" s="74"/>
+      <c r="P36" s="74"/>
+      <c r="Q36" s="74"/>
+      <c r="R36" s="74"/>
+      <c r="S36" s="74"/>
+      <c r="T36" s="74"/>
+      <c r="U36" s="74"/>
+      <c r="V36" s="74"/>
+      <c r="W36" s="74"/>
+      <c r="X36" s="74"/>
+      <c r="Y36" s="74"/>
+      <c r="Z36" s="74"/>
+      <c r="AA36" s="74"/>
+    </row>
+    <row r="37" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="22"/>
       <c r="B37" s="41" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D37" s="55"/>
       <c r="E37" s="55"/>
@@ -3346,34 +3346,34 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H37" s="79"/>
-      <c r="I37" s="79"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="79"/>
-      <c r="N37" s="79"/>
-      <c r="O37" s="79"/>
-      <c r="P37" s="79"/>
-      <c r="Q37" s="79"/>
-      <c r="R37" s="79"/>
-      <c r="S37" s="79"/>
-      <c r="T37" s="79"/>
-      <c r="U37" s="79"/>
-      <c r="V37" s="79"/>
-      <c r="W37" s="79"/>
-      <c r="X37" s="79"/>
-      <c r="Y37" s="79"/>
-      <c r="Z37" s="79"/>
-      <c r="AA37" s="79"/>
-    </row>
-    <row r="38" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H37" s="74"/>
+      <c r="I37" s="74"/>
+      <c r="J37" s="74"/>
+      <c r="K37" s="74"/>
+      <c r="L37" s="74"/>
+      <c r="M37" s="74"/>
+      <c r="N37" s="74"/>
+      <c r="O37" s="74"/>
+      <c r="P37" s="74"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="74"/>
+      <c r="S37" s="74"/>
+      <c r="T37" s="74"/>
+      <c r="U37" s="74"/>
+      <c r="V37" s="74"/>
+      <c r="W37" s="74"/>
+      <c r="X37" s="74"/>
+      <c r="Y37" s="74"/>
+      <c r="Z37" s="74"/>
+      <c r="AA37" s="74"/>
+    </row>
+    <row r="38" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22"/>
       <c r="B38" s="41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D38" s="55"/>
       <c r="E38" s="55"/>
@@ -3382,34 +3382,34 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H38" s="79"/>
-      <c r="I38" s="79"/>
-      <c r="J38" s="79"/>
-      <c r="K38" s="79"/>
-      <c r="L38" s="79"/>
-      <c r="M38" s="79"/>
-      <c r="N38" s="79"/>
-      <c r="O38" s="79"/>
-      <c r="P38" s="79"/>
-      <c r="Q38" s="79"/>
-      <c r="R38" s="79"/>
-      <c r="S38" s="79"/>
-      <c r="T38" s="79"/>
-      <c r="U38" s="79"/>
-      <c r="V38" s="79"/>
-      <c r="W38" s="79"/>
-      <c r="X38" s="79"/>
-      <c r="Y38" s="79"/>
-      <c r="Z38" s="79"/>
-      <c r="AA38" s="79"/>
-    </row>
-    <row r="39" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="74"/>
+      <c r="L38" s="74"/>
+      <c r="M38" s="74"/>
+      <c r="N38" s="74"/>
+      <c r="O38" s="74"/>
+      <c r="P38" s="74"/>
+      <c r="Q38" s="74"/>
+      <c r="R38" s="74"/>
+      <c r="S38" s="74"/>
+      <c r="T38" s="74"/>
+      <c r="U38" s="74"/>
+      <c r="V38" s="74"/>
+      <c r="W38" s="74"/>
+      <c r="X38" s="74"/>
+      <c r="Y38" s="74"/>
+      <c r="Z38" s="74"/>
+      <c r="AA38" s="74"/>
+    </row>
+    <row r="39" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="22"/>
       <c r="B39" s="41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D39" s="55"/>
       <c r="E39" s="55"/>
@@ -3418,33 +3418,33 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H39" s="79"/>
-      <c r="I39" s="79"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="79"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79"/>
-      <c r="N39" s="79"/>
-      <c r="O39" s="79"/>
-      <c r="P39" s="79"/>
-      <c r="Q39" s="79"/>
-      <c r="R39" s="79"/>
-      <c r="S39" s="79"/>
-      <c r="T39" s="79"/>
-      <c r="U39" s="79"/>
-      <c r="V39" s="79"/>
-      <c r="W39" s="79"/>
-      <c r="X39" s="79"/>
-      <c r="Y39" s="79"/>
-      <c r="Z39" s="79"/>
-      <c r="AA39" s="79"/>
-    </row>
-    <row r="40" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H39" s="74"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="74"/>
+      <c r="K39" s="74"/>
+      <c r="L39" s="74"/>
+      <c r="M39" s="74"/>
+      <c r="N39" s="74"/>
+      <c r="O39" s="74"/>
+      <c r="P39" s="74"/>
+      <c r="Q39" s="74"/>
+      <c r="R39" s="74"/>
+      <c r="S39" s="74"/>
+      <c r="T39" s="74"/>
+      <c r="U39" s="74"/>
+      <c r="V39" s="74"/>
+      <c r="W39" s="74"/>
+      <c r="X39" s="74"/>
+      <c r="Y39" s="74"/>
+      <c r="Z39" s="74"/>
+      <c r="AA39" s="74"/>
+    </row>
+    <row r="40" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C40" s="66"/>
       <c r="D40" s="67"/>
@@ -3454,129 +3454,129 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H40" s="80"/>
-      <c r="I40" s="80"/>
-      <c r="J40" s="80"/>
-      <c r="K40" s="80"/>
-      <c r="L40" s="80"/>
-      <c r="M40" s="80"/>
-      <c r="N40" s="80"/>
-      <c r="O40" s="80"/>
-      <c r="P40" s="80"/>
-      <c r="Q40" s="80"/>
-      <c r="R40" s="80"/>
-      <c r="S40" s="80"/>
-      <c r="T40" s="80"/>
-      <c r="U40" s="79"/>
-      <c r="V40" s="79"/>
-      <c r="W40" s="79"/>
-      <c r="X40" s="79"/>
-      <c r="Y40" s="79"/>
-      <c r="Z40" s="79"/>
-      <c r="AA40" s="79"/>
-    </row>
-    <row r="41" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H40" s="75"/>
+      <c r="I40" s="75"/>
+      <c r="J40" s="75"/>
+      <c r="K40" s="75"/>
+      <c r="L40" s="75"/>
+      <c r="M40" s="75"/>
+      <c r="N40" s="75"/>
+      <c r="O40" s="75"/>
+      <c r="P40" s="75"/>
+      <c r="Q40" s="75"/>
+      <c r="R40" s="75"/>
+      <c r="S40" s="75"/>
+      <c r="T40" s="75"/>
+      <c r="U40" s="74"/>
+      <c r="V40" s="74"/>
+      <c r="W40" s="74"/>
+      <c r="X40" s="74"/>
+      <c r="Y40" s="74"/>
+      <c r="Z40" s="74"/>
+      <c r="AA40" s="74"/>
+    </row>
+    <row r="41" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22"/>
       <c r="B41" s="69" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C41" s="70" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D41" s="71"/>
       <c r="E41" s="71"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
-      <c r="H41" s="79"/>
-      <c r="I41" s="79"/>
-      <c r="J41" s="79"/>
-      <c r="K41" s="79"/>
-      <c r="L41" s="79"/>
-      <c r="M41" s="79"/>
-      <c r="N41" s="79"/>
-      <c r="O41" s="79"/>
-      <c r="P41" s="79"/>
-      <c r="Q41" s="79"/>
-      <c r="R41" s="79"/>
-      <c r="S41" s="79"/>
-      <c r="T41" s="79"/>
-      <c r="U41" s="79"/>
-      <c r="V41" s="79"/>
-      <c r="W41" s="79"/>
-      <c r="X41" s="79"/>
-      <c r="Y41" s="79"/>
-      <c r="Z41" s="79"/>
-      <c r="AA41" s="79"/>
-    </row>
-    <row r="42" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H41" s="74"/>
+      <c r="I41" s="74"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="74"/>
+      <c r="L41" s="74"/>
+      <c r="M41" s="74"/>
+      <c r="N41" s="74"/>
+      <c r="O41" s="74"/>
+      <c r="P41" s="74"/>
+      <c r="Q41" s="74"/>
+      <c r="R41" s="74"/>
+      <c r="S41" s="74"/>
+      <c r="T41" s="74"/>
+      <c r="U41" s="74"/>
+      <c r="V41" s="74"/>
+      <c r="W41" s="74"/>
+      <c r="X41" s="74"/>
+      <c r="Y41" s="74"/>
+      <c r="Z41" s="74"/>
+      <c r="AA41" s="74"/>
+    </row>
+    <row r="42" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="22"/>
       <c r="B42" s="69" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C42" s="70" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D42" s="71"/>
       <c r="E42" s="71"/>
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
-      <c r="H42" s="79"/>
-      <c r="I42" s="79"/>
-      <c r="J42" s="79"/>
-      <c r="K42" s="79"/>
-      <c r="L42" s="79"/>
-      <c r="M42" s="79"/>
-      <c r="N42" s="79"/>
-      <c r="O42" s="79"/>
-      <c r="P42" s="79"/>
-      <c r="Q42" s="79"/>
-      <c r="R42" s="79"/>
-      <c r="S42" s="79"/>
-      <c r="T42" s="79"/>
-      <c r="U42" s="79"/>
-      <c r="V42" s="79"/>
-      <c r="W42" s="79"/>
-      <c r="X42" s="79"/>
-      <c r="Y42" s="79"/>
-      <c r="Z42" s="79"/>
-      <c r="AA42" s="79"/>
-    </row>
-    <row r="43" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="74"/>
+      <c r="K42" s="74"/>
+      <c r="L42" s="74"/>
+      <c r="M42" s="74"/>
+      <c r="N42" s="74"/>
+      <c r="O42" s="74"/>
+      <c r="P42" s="74"/>
+      <c r="Q42" s="74"/>
+      <c r="R42" s="74"/>
+      <c r="S42" s="74"/>
+      <c r="T42" s="74"/>
+      <c r="U42" s="74"/>
+      <c r="V42" s="74"/>
+      <c r="W42" s="74"/>
+      <c r="X42" s="74"/>
+      <c r="Y42" s="74"/>
+      <c r="Z42" s="74"/>
+      <c r="AA42" s="74"/>
+    </row>
+    <row r="43" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="22"/>
       <c r="B43" s="69" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C43" s="70" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D43" s="71"/>
       <c r="E43" s="71"/>
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="79"/>
-      <c r="J43" s="79"/>
-      <c r="K43" s="79"/>
-      <c r="L43" s="79"/>
-      <c r="M43" s="79"/>
-      <c r="N43" s="79"/>
-      <c r="O43" s="79"/>
-      <c r="P43" s="79"/>
-      <c r="Q43" s="79"/>
-      <c r="R43" s="79"/>
-      <c r="S43" s="79"/>
-      <c r="T43" s="79"/>
-      <c r="U43" s="79"/>
-      <c r="V43" s="79"/>
-      <c r="W43" s="79"/>
-      <c r="X43" s="79"/>
-      <c r="Y43" s="79"/>
-      <c r="Z43" s="79"/>
-      <c r="AA43" s="79"/>
-    </row>
-    <row r="44" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H43" s="74"/>
+      <c r="I43" s="74"/>
+      <c r="J43" s="74"/>
+      <c r="K43" s="74"/>
+      <c r="L43" s="74"/>
+      <c r="M43" s="74"/>
+      <c r="N43" s="74"/>
+      <c r="O43" s="74"/>
+      <c r="P43" s="74"/>
+      <c r="Q43" s="74"/>
+      <c r="R43" s="74"/>
+      <c r="S43" s="74"/>
+      <c r="T43" s="74"/>
+      <c r="U43" s="74"/>
+      <c r="V43" s="74"/>
+      <c r="W43" s="74"/>
+      <c r="X43" s="74"/>
+      <c r="Y43" s="74"/>
+      <c r="Z43" s="74"/>
+      <c r="AA43" s="74"/>
+    </row>
+    <row r="44" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B44" s="42"/>
       <c r="C44" s="37"/>
@@ -3587,33 +3587,33 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H44" s="79"/>
-      <c r="I44" s="79"/>
-      <c r="J44" s="79"/>
-      <c r="K44" s="79"/>
-      <c r="L44" s="79"/>
-      <c r="M44" s="79"/>
-      <c r="N44" s="79"/>
-      <c r="O44" s="79"/>
-      <c r="P44" s="79"/>
-      <c r="Q44" s="79"/>
-      <c r="R44" s="79"/>
-      <c r="S44" s="79"/>
-      <c r="T44" s="79"/>
-      <c r="U44" s="79"/>
-      <c r="V44" s="79"/>
-      <c r="W44" s="79"/>
-      <c r="X44" s="79"/>
-      <c r="Y44" s="79"/>
-      <c r="Z44" s="79"/>
-      <c r="AA44" s="79"/>
-    </row>
-    <row r="45" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H44" s="74"/>
+      <c r="I44" s="74"/>
+      <c r="J44" s="74"/>
+      <c r="K44" s="74"/>
+      <c r="L44" s="74"/>
+      <c r="M44" s="74"/>
+      <c r="N44" s="74"/>
+      <c r="O44" s="74"/>
+      <c r="P44" s="74"/>
+      <c r="Q44" s="74"/>
+      <c r="R44" s="74"/>
+      <c r="S44" s="74"/>
+      <c r="T44" s="74"/>
+      <c r="U44" s="74"/>
+      <c r="V44" s="74"/>
+      <c r="W44" s="74"/>
+      <c r="X44" s="74"/>
+      <c r="Y44" s="74"/>
+      <c r="Z44" s="74"/>
+      <c r="AA44" s="74"/>
+    </row>
+    <row r="45" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="57"/>
@@ -3623,35 +3623,35 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H45" s="84"/>
-      <c r="I45" s="84"/>
-      <c r="J45" s="84"/>
-      <c r="K45" s="84"/>
-      <c r="L45" s="84"/>
-      <c r="M45" s="84"/>
-      <c r="N45" s="84"/>
-      <c r="O45" s="84"/>
-      <c r="P45" s="84"/>
-      <c r="Q45" s="84"/>
-      <c r="R45" s="84"/>
-      <c r="S45" s="84"/>
-      <c r="T45" s="84"/>
-      <c r="U45" s="84"/>
-      <c r="V45" s="84"/>
-      <c r="W45" s="84"/>
-      <c r="X45" s="84"/>
-      <c r="Y45" s="84"/>
-      <c r="Z45" s="84"/>
-      <c r="AA45" s="84"/>
-    </row>
-    <row r="46" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H45" s="79"/>
+      <c r="I45" s="79"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="79"/>
+      <c r="M45" s="79"/>
+      <c r="N45" s="79"/>
+      <c r="O45" s="79"/>
+      <c r="P45" s="79"/>
+      <c r="Q45" s="79"/>
+      <c r="R45" s="79"/>
+      <c r="S45" s="79"/>
+      <c r="T45" s="79"/>
+      <c r="U45" s="79"/>
+      <c r="V45" s="79"/>
+      <c r="W45" s="79"/>
+      <c r="X45" s="79"/>
+      <c r="Y45" s="79"/>
+      <c r="Z45" s="79"/>
+      <c r="AA45" s="79"/>
+    </row>
+    <row r="46" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="11"/>
       <c r="E47" s="24"/>
     </row>
-    <row r="48" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="12"/>
     </row>
   </sheetData>
@@ -3697,7 +3697,7 @@
       <formula>AND(TODAY()&gt;=AA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Mostrar semana" prompt="Al cambiar este número, se desplazará la vista del diagrama de Gantt." sqref="D4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
@@ -3713,6 +3713,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100CE8683845CA09544BDD5D2CFA119F453" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="25e64108eeebe26551eee07707bcd7de">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="490ce474-600e-4e79-85eb-56e37e2f143b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="23adf563ecffdbcf6d9713f65d527ff9" ns2:_="">
     <xsd:import namespace="490ce474-600e-4e79-85eb-56e37e2f143b"/>
@@ -3856,22 +3871,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3471B813-2B12-46F0-BD03-DECCBFECE95B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3887,21 +3904,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Añadido el Rag Asincrono y Prepado para Mergear Main
</commit_message>
<xml_diff>
--- a/documentación/Plantilla Diagrama de Gantt.xlsx
+++ b/documentación/Plantilla Diagrama de Gantt.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27729"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222422F2-AC2F-482A-865D-B882646781E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="241" documentId="13_ncr:1_{222422F2-AC2F-482A-865D-B882646781E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E129E45-8FC6-4B70-8EF4-7B2E7C63D532}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -48,7 +48,13 @@
 Desplácese hacia abajo por la columna A para escuchar más instrucciones.</t>
   </si>
   <si>
+    <t>ChatBOC</t>
+  </si>
+  <si>
     <t>Escriba el nombre de la compañía en la celda B2.</t>
+  </si>
+  <si>
+    <t>Nombre del equipo: "Equipo A".</t>
   </si>
   <si>
     <t>Escriba el nombre del responsable del proyecto en la celda B3. Escriba la fecha de comienzo del proyecto en la celda E3. Inicio del proyecto: la etiqueta se encuentra en la celda C3.</t>
@@ -120,6 +126,12 @@
 Para eliminar la fase y trabajar solo con las tareas, elimine esta fila.</t>
   </si>
   <si>
+    <t>Scrapping y Vectorización (Embedding)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
     <t xml:space="preserve">La celda B9 contiene la tarea de ejemplo "Tarea 1". 
 Escriba un nuevo nombre de tarea en la celda B9.
 Escriba una persona a la que asignar la tarea en la celda C9.
@@ -129,6 +141,12 @@
 Aparece una barra de estado con sombreado para las fechas especificadas en bloques comenzando desde la celda I9 hasta la BL9. </t>
   </si>
   <si>
+    <t>Clase Scrapping</t>
+  </si>
+  <si>
+    <t>JR</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -136,6 +154,36 @@
 Repita las instrucciones de la celda A9 para todas las filas de tareas en esta hoja de cálculo. Sobrescriba los datos de ejemplo.
 Un ejemplo de otra fase empieza en la celda A14. 
 Continue escribiendo tareas en las celdas de la A10 a la A13 o vaya a la celda A14 para obtener más información.</t>
+  </si>
+  <si>
+    <t>Clase Conversión PDF a TXT</t>
+  </si>
+  <si>
+    <t>Clase BDChroma</t>
+  </si>
+  <si>
+    <t>Aarón y JR</t>
+  </si>
+  <si>
+    <t>Docker Chroma BD</t>
+  </si>
+  <si>
+    <t>Manolo</t>
+  </si>
+  <si>
+    <t>Scrapping diario</t>
+  </si>
+  <si>
+    <t>Crear app Main Scrapper</t>
+  </si>
+  <si>
+    <t>Integración PDFs diarios BD</t>
+  </si>
+  <si>
+    <t>Despliege Docker Actions</t>
+  </si>
+  <si>
+    <t>Copia Seguridad PDFs</t>
   </si>
   <si>
     <t>La celda a la derecha contiene el título de ejemplo de la Fase 2. 
@@ -148,7 +196,109 @@
 Repita las instrucciones de las celdas A8 y A9 cuando lo necesite.</t>
   </si>
   <si>
+    <t>Web UI y LLM</t>
+  </si>
+  <si>
+    <t>Docker de Base de datos (User)</t>
+  </si>
+  <si>
+    <t>Docker Ollama</t>
+  </si>
+  <si>
+    <t>Docker Web y LLM</t>
+  </si>
+  <si>
+    <t>BackEnd de control de usuario</t>
+  </si>
+  <si>
+    <t>Aarón</t>
+  </si>
+  <si>
+    <t>UI de acceso (Login)</t>
+  </si>
+  <si>
+    <t>Juan Carlos</t>
+  </si>
+  <si>
+    <t>UI de Registro</t>
+  </si>
+  <si>
+    <t>UI de Chatbot</t>
+  </si>
+  <si>
+    <t>LLM (RAG)</t>
+  </si>
+  <si>
+    <t>Integración UI y LLM (Chatbot)</t>
+  </si>
+  <si>
+    <t>JR y Juan Carlos</t>
+  </si>
+  <si>
+    <t>Integración UI y BD (SQL)</t>
+  </si>
+  <si>
+    <t>Despliegue Sistema Completo</t>
+  </si>
+  <si>
     <t>Bloque de título fase de ejemplo</t>
+  </si>
+  <si>
+    <t>Log y Power BI</t>
+  </si>
+  <si>
+    <t>Clase PowerBi</t>
+  </si>
+  <si>
+    <t>Inyección de LOG (ChatBoc)</t>
+  </si>
+  <si>
+    <t>Preparación Datos Power Bi</t>
+  </si>
+  <si>
+    <t>Iosu</t>
+  </si>
+  <si>
+    <t>Panel de Control Power Bi</t>
+  </si>
+  <si>
+    <t>Documentación</t>
+  </si>
+  <si>
+    <t>Test Unitarios</t>
+  </si>
+  <si>
+    <t>Pruebas del sistema</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Manual de Despliegle</t>
+  </si>
+  <si>
+    <t>Manual de Implementación</t>
+  </si>
+  <si>
+    <t>Manual de Usuario</t>
+  </si>
+  <si>
+    <t>Mejoras (Si nos da tiempo)</t>
+  </si>
+  <si>
+    <t>Docker API-REST</t>
+  </si>
+  <si>
+    <t>API + LLM</t>
+  </si>
+  <si>
+    <t>Despliege en Azure</t>
+  </si>
+  <si>
+    <t>Manolo y JR</t>
+  </si>
+  <si>
+    <t>App Android (Básica)</t>
   </si>
   <si>
     <t>Esta es una fila vacía.</t>
@@ -159,159 +309,6 @@
   </si>
   <si>
     <t>Inserte nuevas filas ENCIMA de ésta</t>
-  </si>
-  <si>
-    <t>Scrapping y Vectorización (embedding)</t>
-  </si>
-  <si>
-    <t>Clase Scrapping</t>
-  </si>
-  <si>
-    <t>Clase Conversión PDF a TXT</t>
-  </si>
-  <si>
-    <t>JR</t>
-  </si>
-  <si>
-    <t>Docker Chrome BD</t>
-  </si>
-  <si>
-    <t>Manolo</t>
-  </si>
-  <si>
-    <t>Juan Carlos y Iosu</t>
-  </si>
-  <si>
-    <t>Scrapping diario</t>
-  </si>
-  <si>
-    <t>Despliege Docker Action</t>
-  </si>
-  <si>
-    <t>Crear app Main Scrapper</t>
-  </si>
-  <si>
-    <t>Iosu</t>
-  </si>
-  <si>
-    <t>Web UI y LLM</t>
-  </si>
-  <si>
-    <t>BackEnd de control de usuario</t>
-  </si>
-  <si>
-    <t>Aaron</t>
-  </si>
-  <si>
-    <t>UI de acceso (login)</t>
-  </si>
-  <si>
-    <t>Juan Carlos</t>
-  </si>
-  <si>
-    <t>UI de Registro</t>
-  </si>
-  <si>
-    <t>UI de ChatBot</t>
-  </si>
-  <si>
-    <t>LLM</t>
-  </si>
-  <si>
-    <t>Integración PDFs díarios BD</t>
-  </si>
-  <si>
-    <t>Log y Power BI</t>
-  </si>
-  <si>
-    <t>Integracición UI y LLM</t>
-  </si>
-  <si>
-    <t>JR y Juan Carlos</t>
-  </si>
-  <si>
-    <t>Clase LOGChatBOC</t>
-  </si>
-  <si>
-    <t>Iosu y Aarón</t>
-  </si>
-  <si>
-    <t>Aarón</t>
-  </si>
-  <si>
-    <t>Aarón y JR</t>
-  </si>
-  <si>
-    <t>Mejoras (Si nos da tiempo)</t>
-  </si>
-  <si>
-    <t>Inyección de LOG (ChatBoc)</t>
-  </si>
-  <si>
-    <t>Documentación</t>
-  </si>
-  <si>
-    <t>Manual de Despliegle</t>
-  </si>
-  <si>
-    <t>Manual de Implementación</t>
-  </si>
-  <si>
-    <t>Manual de Usuario</t>
-  </si>
-  <si>
-    <t>Todos</t>
-  </si>
-  <si>
-    <t>Docker Ollama</t>
-  </si>
-  <si>
-    <t>Docker de Base de datos (User)</t>
-  </si>
-  <si>
-    <t>Docker Web y LLM</t>
-  </si>
-  <si>
-    <t>Iosu y JR</t>
-  </si>
-  <si>
-    <t>Panel de Control Power Bi</t>
-  </si>
-  <si>
-    <t>Preparación Datos Power Bi</t>
-  </si>
-  <si>
-    <t>Test Unitarios</t>
-  </si>
-  <si>
-    <t>Pruebas del sistema</t>
-  </si>
-  <si>
-    <t>JR y Aarón</t>
-  </si>
-  <si>
-    <t>App Android (Básica)</t>
-  </si>
-  <si>
-    <t>Docker API-REST</t>
-  </si>
-  <si>
-    <t>API + LLM</t>
-  </si>
-  <si>
-    <t>Copia Seguridad PDFs</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Clase BDChroma</t>
-  </si>
-  <si>
-    <t>Nombre del equipo: "Equipo A".</t>
-  </si>
-  <si>
-    <t>ChatBOC</t>
   </si>
 </sst>
 </file>
@@ -329,7 +326,7 @@
     <numFmt numFmtId="169" formatCode="d\ &quot;de&quot;\ mmmm"/>
     <numFmt numFmtId="170" formatCode="d\ &quot;de&quot;\ mmmm\ "/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="38">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -560,8 +557,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="51">
+  <fills count="61">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -846,6 +886,66 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0504D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1102,7 +1202,7 @@
     <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1296,12 +1396,6 @@
     <xf numFmtId="166" fontId="5" fillId="48" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="49" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="49" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="9" fillId="49" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1329,7 +1423,76 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="32" fillId="45" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="50" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="45" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="52" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="53" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="54" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="55" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="50" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="49" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="49" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="45" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="56" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="57" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="58" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="59" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="59" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="59" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="60" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1343,6 +1506,9 @@
     </xf>
     <xf numFmtId="169" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1427,6 +1593,17 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -1436,17 +1613,6 @@
         </right>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
       </border>
     </dxf>
     <dxf>
@@ -1997,107 +2163,107 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA48"/>
+  <dimension ref="A1:AA50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="AC39" sqref="AC39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="22" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="3.140625" customWidth="1"/>
     <col min="7" max="7" width="6.140625" hidden="1" customWidth="1"/>
     <col min="8" max="27" width="4" style="5" customWidth="1"/>
     <col min="32" max="33" width="10.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" ht="30" customHeight="1">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="4"/>
       <c r="E1" s="21"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="72"/>
-    </row>
-    <row r="2" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="70"/>
+    </row>
+    <row r="2" spans="1:27" ht="30" customHeight="1">
       <c r="A2" s="22" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="73"/>
-    </row>
-    <row r="3" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H2" s="71"/>
+    </row>
+    <row r="3" spans="1:27" ht="30" customHeight="1">
       <c r="A3" s="22" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="61" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="80">
+        <v>5</v>
+      </c>
+      <c r="D3" s="106">
         <v>45432</v>
       </c>
-      <c r="E3" s="80"/>
-    </row>
-    <row r="4" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="106"/>
+    </row>
+    <row r="4" spans="1:27" ht="30" customHeight="1">
       <c r="A4" s="23" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="H4" s="81">
+      <c r="H4" s="102">
         <f>H5</f>
         <v>45432</v>
       </c>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="81">
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="102">
         <f>H5+7</f>
         <v>45439</v>
       </c>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="83">
+      <c r="N4" s="103"/>
+      <c r="O4" s="103"/>
+      <c r="P4" s="103"/>
+      <c r="Q4" s="103"/>
+      <c r="R4" s="104">
         <f>H5+14</f>
         <v>45446</v>
       </c>
-      <c r="S4" s="84"/>
-      <c r="T4" s="84"/>
-      <c r="U4" s="84"/>
-      <c r="V4" s="84"/>
-      <c r="W4" s="83">
+      <c r="S4" s="105"/>
+      <c r="T4" s="105"/>
+      <c r="U4" s="105"/>
+      <c r="V4" s="105"/>
+      <c r="W4" s="104">
         <f>H5+21</f>
         <v>45453</v>
       </c>
-      <c r="X4" s="84"/>
-      <c r="Y4" s="84"/>
-      <c r="Z4" s="84"/>
-      <c r="AA4" s="84"/>
-    </row>
-    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X4" s="105"/>
+      <c r="Y4" s="105"/>
+      <c r="Z4" s="105"/>
+      <c r="AA4" s="105"/>
+    </row>
+    <row r="5" spans="1:27" ht="15" customHeight="1">
       <c r="A5" s="23" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
@@ -2185,25 +2351,25 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" ht="30" customHeight="1" thickBot="1">
       <c r="A6" s="23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H6" s="10" t="str">
         <f t="shared" ref="H6" si="1">LEFT(TEXT(H5,"ddd"),1)</f>
@@ -2214,7 +2380,7 @@
         <v>m</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K6" s="10" t="str">
         <f>LEFT(TEXT(K5,"ddd"),1)</f>
@@ -2225,238 +2391,247 @@
         <v>v</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="P6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="S6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="S6" s="10" t="s">
+      <c r="T6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="T6" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="U6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="W6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="V6" s="10" t="s">
+      <c r="X6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="W6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="X6" s="10" t="s">
+      <c r="Y6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="Y6" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="Z6" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AA6" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A7" s="22" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7"/>
       <c r="G7" t="str">
-        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f ca="1">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="74"/>
-      <c r="T7" s="74"/>
-      <c r="U7" s="74"/>
-      <c r="V7" s="74"/>
-      <c r="W7" s="74"/>
-      <c r="X7" s="74"/>
-      <c r="Y7" s="74"/>
-      <c r="Z7" s="74"/>
-      <c r="AA7" s="74"/>
-    </row>
-    <row r="8" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="72"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="72"/>
+      <c r="Q7" s="72"/>
+      <c r="R7" s="72"/>
+      <c r="S7" s="72"/>
+      <c r="T7" s="72"/>
+      <c r="U7" s="72"/>
+      <c r="V7" s="72"/>
+      <c r="W7" s="72"/>
+      <c r="X7" s="72"/>
+      <c r="Y7" s="72"/>
+      <c r="Z7" s="72"/>
+      <c r="AA7" s="72"/>
+    </row>
+    <row r="8" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A8" s="23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C8" s="29"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45"/>
+      <c r="D8" s="44">
+        <v>45432</v>
+      </c>
+      <c r="E8" s="45">
+        <v>45448</v>
+      </c>
       <c r="F8" s="63"/>
       <c r="G8" s="63"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="75"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="75"/>
-      <c r="Q8" s="75"/>
-      <c r="R8" s="75"/>
-      <c r="S8" s="75"/>
-      <c r="T8" s="75"/>
-      <c r="U8" s="74"/>
-      <c r="V8" s="74"/>
-      <c r="W8" s="74"/>
-      <c r="X8" s="74"/>
-      <c r="Y8" s="74"/>
-      <c r="Z8" s="74"/>
-      <c r="AA8" s="74"/>
-    </row>
-    <row r="9" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
+      <c r="M8" s="101"/>
+      <c r="N8" s="101"/>
+      <c r="O8" s="101"/>
+      <c r="P8" s="101"/>
+      <c r="Q8" s="101"/>
+      <c r="R8" s="101"/>
+      <c r="S8" s="101"/>
+      <c r="T8" s="101" t="s">
+        <v>23</v>
+      </c>
+      <c r="U8" s="72"/>
+      <c r="V8" s="72"/>
+      <c r="W8" s="72"/>
+      <c r="X8" s="72"/>
+      <c r="Y8" s="72"/>
+      <c r="Z8" s="72"/>
+      <c r="AA8" s="72"/>
+    </row>
+    <row r="9" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A9" s="23" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D9" s="46">
         <f>Inicio_del_proyecto</f>
         <v>45432</v>
       </c>
       <c r="E9" s="46">
-        <v>45433</v>
+        <v>45434</v>
       </c>
       <c r="F9" s="64"/>
       <c r="G9" s="64"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="75"/>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="75"/>
-      <c r="S9" s="75"/>
-      <c r="T9" s="75"/>
-      <c r="U9" s="74"/>
-      <c r="V9" s="74"/>
-      <c r="W9" s="74"/>
-      <c r="X9" s="74" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y9" s="74"/>
-      <c r="Z9" s="74"/>
-      <c r="AA9" s="74"/>
-    </row>
-    <row r="10" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="73"/>
+      <c r="T9" s="73"/>
+      <c r="U9" s="72"/>
+      <c r="V9" s="72"/>
+      <c r="W9" s="72"/>
+      <c r="X9" s="72" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y9" s="72"/>
+      <c r="Z9" s="72"/>
+      <c r="AA9" s="72"/>
+    </row>
+    <row r="10" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A10" s="23" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D10" s="46">
         <f>Inicio_del_proyecto</f>
         <v>45432</v>
       </c>
       <c r="E10" s="46">
-        <v>45433</v>
+        <v>45434</v>
       </c>
       <c r="F10" s="63"/>
       <c r="G10" s="63"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="75"/>
-      <c r="P10" s="75"/>
-      <c r="Q10" s="75"/>
-      <c r="R10" s="75"/>
-      <c r="S10" s="75"/>
-      <c r="T10" s="75"/>
-      <c r="U10" s="74"/>
-      <c r="V10" s="74"/>
-      <c r="W10" s="74"/>
-      <c r="X10" s="74"/>
-      <c r="Y10" s="74"/>
-      <c r="Z10" s="74"/>
-      <c r="AA10" s="74"/>
-    </row>
-    <row r="11" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73"/>
+      <c r="R10" s="73"/>
+      <c r="S10" s="73"/>
+      <c r="T10" s="73"/>
+      <c r="U10" s="72"/>
+      <c r="V10" s="72"/>
+      <c r="W10" s="72"/>
+      <c r="X10" s="72"/>
+      <c r="Y10" s="72"/>
+      <c r="Z10" s="72"/>
+      <c r="AA10" s="72"/>
+    </row>
+    <row r="11" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A11" s="22"/>
       <c r="B11" s="38" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D11" s="46">
-        <f>Inicio_del_proyecto</f>
-        <v>45432</v>
-      </c>
-      <c r="E11" s="46"/>
+        <v>45434</v>
+      </c>
+      <c r="E11" s="46">
+        <v>45440</v>
+      </c>
       <c r="F11" s="63"/>
       <c r="G11" s="63"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="75"/>
-      <c r="P11" s="75"/>
-      <c r="Q11" s="75"/>
-      <c r="R11" s="75"/>
-      <c r="S11" s="75"/>
-      <c r="T11" s="75"/>
-      <c r="U11" s="74"/>
-      <c r="V11" s="74"/>
-      <c r="W11" s="74"/>
-      <c r="X11" s="74"/>
-      <c r="Y11" s="74"/>
-      <c r="Z11" s="74"/>
-      <c r="AA11" s="74"/>
-    </row>
-    <row r="12" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="73"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="74"/>
+      <c r="N11" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="73"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="73"/>
+      <c r="R11" s="73"/>
+      <c r="S11" s="73"/>
+      <c r="T11" s="73"/>
+      <c r="U11" s="72"/>
+      <c r="V11" s="72"/>
+      <c r="W11" s="72"/>
+      <c r="X11" s="72"/>
+      <c r="Y11" s="72"/>
+      <c r="Z11" s="72"/>
+      <c r="AA11" s="72"/>
+    </row>
+    <row r="12" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A12" s="22"/>
       <c r="B12" s="38" t="s">
         <v>32</v>
@@ -2465,850 +2640,990 @@
         <v>33</v>
       </c>
       <c r="D12" s="46">
-        <f>Inicio_del_proyecto</f>
         <v>45432</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="46">
+        <v>45432</v>
+      </c>
       <c r="F12" s="63"/>
       <c r="G12" s="63"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75"/>
-      <c r="L12" s="75"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="75"/>
-      <c r="O12" s="75"/>
-      <c r="P12" s="75"/>
-      <c r="Q12" s="75"/>
-      <c r="R12" s="75"/>
-      <c r="S12" s="75"/>
-      <c r="T12" s="75"/>
-      <c r="U12" s="74"/>
-      <c r="V12" s="74"/>
-      <c r="W12" s="74"/>
-      <c r="X12" s="74"/>
-      <c r="Y12" s="74"/>
-      <c r="Z12" s="74"/>
-      <c r="AA12" s="74"/>
-    </row>
-    <row r="13" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="73"/>
+      <c r="R12" s="73"/>
+      <c r="S12" s="73"/>
+      <c r="T12" s="73"/>
+      <c r="U12" s="72"/>
+      <c r="V12" s="72"/>
+      <c r="W12" s="72"/>
+      <c r="X12" s="72"/>
+      <c r="Y12" s="72"/>
+      <c r="Z12" s="72"/>
+      <c r="AA12" s="72"/>
+    </row>
+    <row r="13" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="22"/>
       <c r="B13" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D13" s="46">
-        <f>Inicio_del_proyecto</f>
-        <v>45432</v>
-      </c>
-      <c r="E13" s="46"/>
+        <v>45434</v>
+      </c>
+      <c r="E13" s="46">
+        <v>45442</v>
+      </c>
       <c r="F13" s="63"/>
       <c r="G13" s="63"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
-      <c r="L13" s="75"/>
-      <c r="M13" s="75"/>
-      <c r="N13" s="75"/>
-      <c r="O13" s="75"/>
-      <c r="P13" s="75"/>
-      <c r="Q13" s="75"/>
-      <c r="R13" s="75"/>
-      <c r="S13" s="75"/>
-      <c r="T13" s="75"/>
-      <c r="U13" s="74"/>
-      <c r="V13" s="74"/>
-      <c r="W13" s="74"/>
-      <c r="X13" s="74"/>
-      <c r="Y13" s="74"/>
-      <c r="Z13" s="74"/>
-      <c r="AA13" s="74"/>
-    </row>
-    <row r="14" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
+      <c r="P13" s="82" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q13" s="73"/>
+      <c r="R13" s="73"/>
+      <c r="S13" s="73"/>
+      <c r="T13" s="73"/>
+      <c r="U13" s="72"/>
+      <c r="V13" s="72"/>
+      <c r="W13" s="72"/>
+      <c r="X13" s="72"/>
+      <c r="Y13" s="72"/>
+      <c r="Z13" s="72"/>
+      <c r="AA13" s="72"/>
+    </row>
+    <row r="14" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A14" s="22"/>
       <c r="B14" s="38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
+        <v>26</v>
+      </c>
+      <c r="D14" s="46">
+        <v>45441</v>
+      </c>
+      <c r="E14" s="46">
+        <v>45443</v>
+      </c>
       <c r="F14" s="63"/>
       <c r="G14" s="63"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="75"/>
-      <c r="M14" s="75"/>
-      <c r="N14" s="75"/>
-      <c r="O14" s="75"/>
-      <c r="P14" s="75"/>
-      <c r="Q14" s="75"/>
-      <c r="R14" s="75"/>
-      <c r="S14" s="75"/>
-      <c r="T14" s="75"/>
-      <c r="U14" s="74"/>
-      <c r="V14" s="74"/>
-      <c r="W14" s="74"/>
-      <c r="X14" s="74"/>
-      <c r="Y14" s="74"/>
-      <c r="Z14" s="74"/>
-      <c r="AA14" s="74"/>
-    </row>
-    <row r="15" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="73"/>
+      <c r="I14" s="73"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="73"/>
+      <c r="L14" s="73"/>
+      <c r="M14" s="73"/>
+      <c r="N14" s="73"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="82" t="s">
+        <v>23</v>
+      </c>
+      <c r="R14" s="73"/>
+      <c r="S14" s="73"/>
+      <c r="T14" s="73"/>
+      <c r="U14" s="72"/>
+      <c r="V14" s="72"/>
+      <c r="W14" s="72"/>
+      <c r="X14" s="72"/>
+      <c r="Y14" s="72"/>
+      <c r="Z14" s="72"/>
+      <c r="AA14" s="72"/>
+    </row>
+    <row r="15" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A15" s="22"/>
       <c r="B15" s="38" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
+        <v>26</v>
+      </c>
+      <c r="D15" s="46">
+        <v>45441</v>
+      </c>
+      <c r="E15" s="46">
+        <v>45443</v>
+      </c>
       <c r="F15" s="63"/>
       <c r="G15" s="63"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="75"/>
-      <c r="L15" s="75"/>
-      <c r="M15" s="75"/>
-      <c r="N15" s="75"/>
-      <c r="O15" s="75"/>
-      <c r="P15" s="75"/>
-      <c r="Q15" s="75"/>
-      <c r="R15" s="75"/>
-      <c r="S15" s="75"/>
-      <c r="T15" s="75"/>
-      <c r="U15" s="74"/>
-      <c r="V15" s="74"/>
-      <c r="W15" s="74"/>
-      <c r="X15" s="74"/>
-      <c r="Y15" s="74"/>
-      <c r="Z15" s="74"/>
-      <c r="AA15" s="74"/>
-    </row>
-    <row r="16" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="82"/>
+      <c r="Q15" s="82" t="s">
+        <v>23</v>
+      </c>
+      <c r="R15" s="73"/>
+      <c r="S15" s="73"/>
+      <c r="T15" s="73"/>
+      <c r="U15" s="72"/>
+      <c r="V15" s="72"/>
+      <c r="W15" s="72"/>
+      <c r="X15" s="72"/>
+      <c r="Y15" s="72"/>
+      <c r="Z15" s="72"/>
+      <c r="AA15" s="72"/>
+    </row>
+    <row r="16" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A16" s="22"/>
       <c r="B16" s="38" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
+      <c r="D16" s="46">
+        <v>45436</v>
+      </c>
+      <c r="E16" s="46">
+        <v>45447</v>
+      </c>
       <c r="F16" s="63"/>
       <c r="G16" s="63"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="75"/>
-      <c r="M16" s="75"/>
-      <c r="N16" s="75"/>
-      <c r="O16" s="75"/>
-      <c r="P16" s="75"/>
-      <c r="Q16" s="75"/>
-      <c r="R16" s="75"/>
-      <c r="S16" s="75"/>
-      <c r="T16" s="75"/>
-      <c r="U16" s="74"/>
-      <c r="V16" s="74"/>
-      <c r="W16" s="74"/>
-      <c r="X16" s="74"/>
-      <c r="Y16" s="74"/>
-      <c r="Z16" s="74"/>
-      <c r="AA16" s="74"/>
-    </row>
-    <row r="17" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="73"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
+      <c r="L16" s="98"/>
+      <c r="M16" s="98"/>
+      <c r="N16" s="96"/>
+      <c r="O16" s="96"/>
+      <c r="P16" s="96"/>
+      <c r="Q16" s="96"/>
+      <c r="R16" s="96"/>
+      <c r="S16" s="97" t="s">
+        <v>23</v>
+      </c>
+      <c r="T16" s="73"/>
+      <c r="U16" s="72"/>
+      <c r="V16" s="72"/>
+      <c r="W16" s="72"/>
+      <c r="X16" s="72"/>
+      <c r="Y16" s="72"/>
+      <c r="Z16" s="72"/>
+      <c r="AA16" s="72"/>
+    </row>
+    <row r="17" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="22"/>
       <c r="B17" s="38" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
+      <c r="D17" s="46">
+        <v>45437</v>
+      </c>
+      <c r="E17" s="46">
+        <v>45448</v>
+      </c>
       <c r="F17" s="63"/>
       <c r="G17" s="63"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="75"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="75"/>
-      <c r="P17" s="75"/>
-      <c r="Q17" s="75"/>
-      <c r="R17" s="75"/>
-      <c r="S17" s="75"/>
-      <c r="T17" s="75"/>
-      <c r="U17" s="74"/>
-      <c r="V17" s="74"/>
-      <c r="W17" s="74"/>
-      <c r="X17" s="74"/>
-      <c r="Y17" s="74"/>
-      <c r="Z17" s="74"/>
-      <c r="AA17" s="74"/>
-    </row>
-    <row r="18" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="98"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="98"/>
+      <c r="O17" s="98"/>
+      <c r="P17" s="98"/>
+      <c r="Q17" s="98"/>
+      <c r="R17" s="98"/>
+      <c r="S17" s="98"/>
+      <c r="T17" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="U17" s="72"/>
+      <c r="V17" s="72"/>
+      <c r="W17" s="72"/>
+      <c r="X17" s="72"/>
+      <c r="Y17" s="72"/>
+      <c r="Z17" s="72"/>
+      <c r="AA17" s="72"/>
+    </row>
+    <row r="18" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A18" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="47">
+        <v>45432</v>
+      </c>
+      <c r="E18" s="48">
+        <v>45448</v>
+      </c>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63">
+        <f t="shared" ref="G18:G47" ca="1" si="3">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>17</v>
+      </c>
+      <c r="H18" s="101"/>
+      <c r="I18" s="101"/>
+      <c r="J18" s="101"/>
+      <c r="K18" s="101"/>
+      <c r="L18" s="101"/>
+      <c r="M18" s="101"/>
+      <c r="N18" s="101"/>
+      <c r="O18" s="101"/>
+      <c r="P18" s="101"/>
+      <c r="Q18" s="101"/>
+      <c r="R18" s="101"/>
+      <c r="S18" s="101"/>
+      <c r="T18" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63" t="str">
-        <f t="shared" ref="G18:G45" si="3">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v/>
-      </c>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
-      <c r="Q18" s="75"/>
-      <c r="R18" s="75"/>
-      <c r="S18" s="75"/>
-      <c r="T18" s="75"/>
-      <c r="U18" s="74"/>
-      <c r="V18" s="74"/>
-      <c r="W18" s="74"/>
-      <c r="X18" s="74"/>
-      <c r="Y18" s="74"/>
-      <c r="Z18" s="74"/>
-      <c r="AA18" s="74"/>
-    </row>
-    <row r="19" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U18" s="72"/>
+      <c r="V18" s="72"/>
+      <c r="W18" s="72"/>
+      <c r="X18" s="72"/>
+      <c r="Y18" s="72"/>
+      <c r="Z18" s="72"/>
+      <c r="AA18" s="72"/>
+    </row>
+    <row r="19" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A19" s="23"/>
       <c r="B19" s="39" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C19" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
+      <c r="D19" s="49">
+        <v>45432</v>
+      </c>
+      <c r="E19" s="49">
+        <v>45432</v>
+      </c>
       <c r="F19" s="63"/>
-      <c r="G19" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="75"/>
-      <c r="P19" s="75"/>
-      <c r="Q19" s="75"/>
-      <c r="R19" s="75"/>
-      <c r="S19" s="75"/>
-      <c r="T19" s="75"/>
-      <c r="U19" s="74"/>
-      <c r="V19" s="74"/>
-      <c r="W19" s="74"/>
-      <c r="X19" s="74"/>
-      <c r="Y19" s="74"/>
-      <c r="Z19" s="74"/>
-      <c r="AA19" s="74"/>
-    </row>
-    <row r="20" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="63">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H19" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="73"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="73"/>
+      <c r="N19" s="73"/>
+      <c r="O19" s="73"/>
+      <c r="P19" s="73"/>
+      <c r="Q19" s="73"/>
+      <c r="R19" s="73"/>
+      <c r="S19" s="73"/>
+      <c r="T19" s="73"/>
+      <c r="U19" s="72"/>
+      <c r="V19" s="72"/>
+      <c r="W19" s="72"/>
+      <c r="X19" s="72"/>
+      <c r="Y19" s="72"/>
+      <c r="Z19" s="72"/>
+      <c r="AA19" s="72"/>
+    </row>
+    <row r="20" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A20" s="23"/>
       <c r="B20" s="39" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C20" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
+      <c r="D20" s="49">
+        <v>45433</v>
+      </c>
+      <c r="E20" s="49">
+        <v>45433</v>
+      </c>
       <c r="F20" s="63"/>
       <c r="G20" s="63"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="75"/>
-      <c r="K20" s="75"/>
-      <c r="L20" s="75"/>
-      <c r="M20" s="75"/>
-      <c r="N20" s="75"/>
-      <c r="O20" s="75"/>
-      <c r="P20" s="75"/>
-      <c r="Q20" s="75"/>
-      <c r="R20" s="75"/>
-      <c r="S20" s="75"/>
-      <c r="T20" s="75"/>
-      <c r="U20" s="74"/>
-      <c r="V20" s="74"/>
-      <c r="W20" s="74"/>
-      <c r="X20" s="74"/>
-      <c r="Y20" s="74"/>
-      <c r="Z20" s="74"/>
-      <c r="AA20" s="74"/>
-    </row>
-    <row r="21" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="73"/>
+      <c r="Q20" s="73"/>
+      <c r="R20" s="73"/>
+      <c r="S20" s="73"/>
+      <c r="T20" s="73"/>
+      <c r="U20" s="72"/>
+      <c r="V20" s="72"/>
+      <c r="W20" s="72"/>
+      <c r="X20" s="72"/>
+      <c r="Y20" s="72"/>
+      <c r="Z20" s="72"/>
+      <c r="AA20" s="72"/>
+    </row>
+    <row r="21" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A21" s="23"/>
       <c r="B21" s="39" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
+      <c r="D21" s="49">
+        <v>45434</v>
+      </c>
+      <c r="E21" s="49">
+        <v>45434</v>
+      </c>
       <c r="F21" s="63"/>
       <c r="G21" s="63"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="75"/>
-      <c r="N21" s="75"/>
-      <c r="O21" s="75"/>
-      <c r="P21" s="75"/>
-      <c r="Q21" s="75"/>
-      <c r="R21" s="75"/>
-      <c r="S21" s="75"/>
-      <c r="T21" s="75"/>
-      <c r="U21" s="74"/>
-      <c r="V21" s="74"/>
-      <c r="W21" s="74"/>
-      <c r="X21" s="74"/>
-      <c r="Y21" s="74"/>
-      <c r="Z21" s="74"/>
-      <c r="AA21" s="74"/>
-    </row>
-    <row r="22" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="73"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="73"/>
+      <c r="Q21" s="73"/>
+      <c r="R21" s="73"/>
+      <c r="S21" s="73"/>
+      <c r="T21" s="73"/>
+      <c r="U21" s="72"/>
+      <c r="V21" s="72"/>
+      <c r="W21" s="72"/>
+      <c r="X21" s="72"/>
+      <c r="Y21" s="72"/>
+      <c r="Z21" s="72"/>
+      <c r="AA21" s="72"/>
+    </row>
+    <row r="22" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A22" s="23"/>
       <c r="B22" s="39" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
+        <v>45</v>
+      </c>
+      <c r="D22" s="49">
+        <v>45433</v>
+      </c>
+      <c r="E22" s="49">
+        <v>45443</v>
+      </c>
       <c r="F22" s="63"/>
-      <c r="G22" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H22" s="75"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="75"/>
-      <c r="M22" s="75"/>
-      <c r="N22" s="75"/>
-      <c r="O22" s="75"/>
-      <c r="P22" s="75"/>
-      <c r="Q22" s="75"/>
-      <c r="R22" s="75"/>
-      <c r="S22" s="75"/>
-      <c r="T22" s="75"/>
-      <c r="U22" s="74"/>
-      <c r="V22" s="74"/>
-      <c r="W22" s="74"/>
-      <c r="X22" s="74"/>
-      <c r="Y22" s="74"/>
-      <c r="Z22" s="74"/>
-      <c r="AA22" s="74"/>
-    </row>
-    <row r="23" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G22" s="63">
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="H22" s="73"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="85"/>
+      <c r="L22" s="85"/>
+      <c r="M22" s="85"/>
+      <c r="N22" s="85"/>
+      <c r="O22" s="85"/>
+      <c r="P22" s="85"/>
+      <c r="Q22" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="R22" s="73"/>
+      <c r="S22" s="73"/>
+      <c r="T22" s="73"/>
+      <c r="U22" s="72"/>
+      <c r="V22" s="72"/>
+      <c r="W22" s="72"/>
+      <c r="X22" s="72"/>
+      <c r="Y22" s="72"/>
+      <c r="Z22" s="72"/>
+      <c r="AA22" s="72"/>
+    </row>
+    <row r="23" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A23" s="22"/>
       <c r="B23" s="39" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
+        <v>47</v>
+      </c>
+      <c r="D23" s="49">
+        <v>45433</v>
+      </c>
+      <c r="E23" s="49">
+        <v>45440</v>
+      </c>
       <c r="F23" s="63"/>
-      <c r="G23" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H23" s="75"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="75"/>
-      <c r="L23" s="75"/>
-      <c r="M23" s="75"/>
-      <c r="N23" s="75"/>
-      <c r="O23" s="75"/>
-      <c r="P23" s="75"/>
-      <c r="Q23" s="75"/>
-      <c r="R23" s="75"/>
-      <c r="S23" s="75"/>
-      <c r="T23" s="75"/>
-      <c r="U23" s="74"/>
-      <c r="V23" s="74"/>
-      <c r="W23" s="74"/>
-      <c r="X23" s="74"/>
-      <c r="Y23" s="74"/>
-      <c r="Z23" s="74"/>
-      <c r="AA23" s="74"/>
-    </row>
-    <row r="24" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G23" s="63">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="H23" s="73"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="84"/>
+      <c r="K23" s="84"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="84"/>
+      <c r="N23" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="O23" s="73"/>
+      <c r="P23" s="73"/>
+      <c r="Q23" s="73"/>
+      <c r="R23" s="73"/>
+      <c r="S23" s="73"/>
+      <c r="T23" s="73"/>
+      <c r="U23" s="72"/>
+      <c r="V23" s="72"/>
+      <c r="W23" s="72"/>
+      <c r="X23" s="72"/>
+      <c r="Y23" s="72"/>
+      <c r="Z23" s="72"/>
+      <c r="AA23" s="72"/>
+    </row>
+    <row r="24" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A24" s="22"/>
       <c r="B24" s="39" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
+        <v>47</v>
+      </c>
+      <c r="D24" s="49">
+        <v>45434</v>
+      </c>
+      <c r="E24" s="49">
+        <v>45441</v>
+      </c>
       <c r="F24" s="63"/>
-      <c r="G24" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="75"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="75"/>
-      <c r="N24" s="75"/>
-      <c r="O24" s="75"/>
-      <c r="P24" s="75"/>
-      <c r="Q24" s="75"/>
-      <c r="R24" s="75"/>
-      <c r="S24" s="75"/>
-      <c r="T24" s="75"/>
-      <c r="U24" s="74"/>
-      <c r="V24" s="74"/>
-      <c r="W24" s="74"/>
-      <c r="X24" s="74"/>
-      <c r="Y24" s="74"/>
-      <c r="Z24" s="74"/>
-      <c r="AA24" s="74"/>
-    </row>
-    <row r="25" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="63">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="H24" s="73"/>
+      <c r="I24" s="84"/>
+      <c r="J24" s="84"/>
+      <c r="K24" s="84"/>
+      <c r="L24" s="84"/>
+      <c r="M24" s="84"/>
+      <c r="N24" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" s="73"/>
+      <c r="P24" s="73"/>
+      <c r="Q24" s="73"/>
+      <c r="R24" s="73"/>
+      <c r="S24" s="73"/>
+      <c r="T24" s="73"/>
+      <c r="U24" s="72"/>
+      <c r="V24" s="72"/>
+      <c r="W24" s="72"/>
+      <c r="X24" s="72"/>
+      <c r="Y24" s="72"/>
+      <c r="Z24" s="72"/>
+      <c r="AA24" s="72"/>
+    </row>
+    <row r="25" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A25" s="22"/>
       <c r="B25" s="39" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
+        <v>47</v>
+      </c>
+      <c r="D25" s="49">
+        <v>45435</v>
+      </c>
+      <c r="E25" s="49">
+        <v>45442</v>
+      </c>
       <c r="F25" s="63"/>
-      <c r="G25" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H25" s="75"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="75"/>
-      <c r="K25" s="75"/>
-      <c r="L25" s="75"/>
-      <c r="M25" s="75"/>
-      <c r="N25" s="75"/>
-      <c r="O25" s="75"/>
-      <c r="P25" s="75"/>
-      <c r="Q25" s="75"/>
-      <c r="R25" s="75"/>
-      <c r="S25" s="75"/>
-      <c r="T25" s="75"/>
-      <c r="U25" s="74"/>
-      <c r="V25" s="74"/>
-      <c r="W25" s="74"/>
-      <c r="X25" s="74"/>
-      <c r="Y25" s="74"/>
-      <c r="Z25" s="74"/>
-      <c r="AA25" s="74"/>
-    </row>
-    <row r="26" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="63">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="H25" s="73"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="84"/>
+      <c r="K25" s="84"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="84"/>
+      <c r="N25" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="O25" s="73"/>
+      <c r="P25" s="73"/>
+      <c r="Q25" s="73"/>
+      <c r="R25" s="73"/>
+      <c r="S25" s="73"/>
+      <c r="T25" s="73"/>
+      <c r="U25" s="72"/>
+      <c r="V25" s="72"/>
+      <c r="W25" s="72"/>
+      <c r="X25" s="72"/>
+      <c r="Y25" s="72"/>
+      <c r="Z25" s="72"/>
+      <c r="AA25" s="72"/>
+    </row>
+    <row r="26" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A26" s="22"/>
       <c r="B26" s="39" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
+        <v>26</v>
+      </c>
+      <c r="D26" s="49">
+        <v>45440</v>
+      </c>
+      <c r="E26" s="49">
+        <v>45441</v>
+      </c>
       <c r="F26" s="63"/>
       <c r="G26" s="63"/>
-      <c r="H26" s="75"/>
-      <c r="I26" s="75"/>
-      <c r="J26" s="75"/>
-      <c r="K26" s="75"/>
-      <c r="L26" s="75"/>
-      <c r="M26" s="75"/>
-      <c r="N26" s="75"/>
-      <c r="O26" s="75"/>
-      <c r="P26" s="75"/>
-      <c r="Q26" s="75"/>
-      <c r="R26" s="75"/>
-      <c r="S26" s="75"/>
-      <c r="T26" s="75"/>
-      <c r="U26" s="74"/>
-      <c r="V26" s="74"/>
-      <c r="W26" s="74"/>
-      <c r="X26" s="74"/>
-      <c r="Y26" s="74"/>
-      <c r="Z26" s="74"/>
-      <c r="AA26" s="74"/>
-    </row>
-    <row r="27" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H26" s="73"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="73"/>
+      <c r="L26" s="73"/>
+      <c r="M26" s="73"/>
+      <c r="N26" s="74"/>
+      <c r="O26" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="P26" s="73"/>
+      <c r="Q26" s="73"/>
+      <c r="R26" s="73"/>
+      <c r="S26" s="73"/>
+      <c r="T26" s="73"/>
+      <c r="U26" s="72"/>
+      <c r="V26" s="72"/>
+      <c r="W26" s="72"/>
+      <c r="X26" s="72"/>
+      <c r="Y26" s="72"/>
+      <c r="Z26" s="72"/>
+      <c r="AA26" s="72"/>
+    </row>
+    <row r="27" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A27" s="22"/>
       <c r="B27" s="39" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
+        <v>52</v>
+      </c>
+      <c r="D27" s="49">
+        <v>45441</v>
+      </c>
+      <c r="E27" s="49">
+        <v>45442</v>
+      </c>
       <c r="F27" s="63"/>
-      <c r="G27" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="75"/>
-      <c r="M27" s="75"/>
-      <c r="N27" s="75"/>
-      <c r="O27" s="75"/>
-      <c r="P27" s="75"/>
-      <c r="Q27" s="75"/>
-      <c r="R27" s="75"/>
-      <c r="S27" s="75"/>
-      <c r="T27" s="75"/>
-      <c r="U27" s="74"/>
-      <c r="V27" s="74"/>
-      <c r="W27" s="74"/>
-      <c r="X27" s="74"/>
-      <c r="Y27" s="74"/>
-      <c r="Z27" s="74"/>
-      <c r="AA27" s="74"/>
-    </row>
-    <row r="28" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="51"/>
+      <c r="G27" s="63">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="H27" s="73"/>
+      <c r="I27" s="73"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="73"/>
+      <c r="M27" s="73"/>
+      <c r="N27" s="73"/>
+      <c r="O27" s="92"/>
+      <c r="P27" s="92" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q27" s="73"/>
+      <c r="R27" s="73"/>
+      <c r="S27" s="73"/>
+      <c r="T27" s="73"/>
+      <c r="U27" s="72"/>
+      <c r="V27" s="72"/>
+      <c r="W27" s="72"/>
+      <c r="X27" s="72"/>
+      <c r="Y27" s="72"/>
+      <c r="Z27" s="72"/>
+      <c r="AA27" s="72"/>
+    </row>
+    <row r="28" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A28" s="22"/>
+      <c r="B28" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="49">
+        <v>45441</v>
+      </c>
+      <c r="E28" s="49">
+        <v>45443</v>
+      </c>
       <c r="F28" s="63"/>
-      <c r="G28" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="75"/>
-      <c r="K28" s="75"/>
-      <c r="L28" s="75"/>
-      <c r="M28" s="75"/>
-      <c r="N28" s="75"/>
-      <c r="O28" s="75"/>
-      <c r="P28" s="75"/>
-      <c r="Q28" s="75"/>
-      <c r="R28" s="75"/>
-      <c r="S28" s="75"/>
-      <c r="T28" s="75"/>
-      <c r="U28" s="74"/>
-      <c r="V28" s="74"/>
-      <c r="W28" s="74"/>
-      <c r="X28" s="74"/>
-      <c r="Y28" s="74"/>
-      <c r="Z28" s="74"/>
-      <c r="AA28" s="74"/>
-    </row>
-    <row r="29" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="63"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="73"/>
+      <c r="L28" s="73"/>
+      <c r="M28" s="73"/>
+      <c r="N28" s="73"/>
+      <c r="O28" s="92"/>
+      <c r="P28" s="92"/>
+      <c r="Q28" s="92" t="s">
+        <v>23</v>
+      </c>
+      <c r="R28" s="73"/>
+      <c r="S28" s="73"/>
+      <c r="T28" s="73"/>
+      <c r="U28" s="72"/>
+      <c r="V28" s="72"/>
+      <c r="W28" s="72"/>
+      <c r="X28" s="72"/>
+      <c r="Y28" s="72"/>
+      <c r="Z28" s="72"/>
+      <c r="AA28" s="72"/>
+    </row>
+    <row r="29" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A29" s="22"/>
-      <c r="B29" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
+      <c r="B29" s="93" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="49">
+        <v>45442</v>
+      </c>
+      <c r="E29" s="49">
+        <v>45446</v>
+      </c>
       <c r="F29" s="63"/>
-      <c r="G29" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H29" s="75"/>
-      <c r="I29" s="75"/>
-      <c r="J29" s="75"/>
-      <c r="K29" s="75"/>
-      <c r="L29" s="75"/>
-      <c r="M29" s="75"/>
-      <c r="N29" s="75"/>
-      <c r="O29" s="75"/>
-      <c r="P29" s="75"/>
-      <c r="Q29" s="75"/>
-      <c r="R29" s="75"/>
-      <c r="S29" s="75"/>
-      <c r="T29" s="75"/>
-      <c r="U29" s="74"/>
-      <c r="V29" s="74"/>
-      <c r="W29" s="74"/>
-      <c r="X29" s="74"/>
-      <c r="Y29" s="74"/>
-      <c r="Z29" s="74"/>
-      <c r="AA29" s="74"/>
-    </row>
-    <row r="30" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
-      <c r="B30" s="40" t="s">
+      <c r="G29" s="63"/>
+      <c r="H29" s="73"/>
+      <c r="I29" s="73"/>
+      <c r="J29" s="73"/>
+      <c r="K29" s="73"/>
+      <c r="L29" s="73"/>
+      <c r="M29" s="73"/>
+      <c r="N29" s="73"/>
+      <c r="O29" s="90"/>
+      <c r="P29" s="95"/>
+      <c r="Q29" s="95"/>
+      <c r="R29" s="95" t="s">
+        <v>23</v>
+      </c>
+      <c r="S29" s="73"/>
+      <c r="T29" s="73"/>
+      <c r="U29" s="72"/>
+      <c r="V29" s="72"/>
+      <c r="W29" s="72"/>
+      <c r="X29" s="72"/>
+      <c r="Y29" s="72"/>
+      <c r="Z29" s="72"/>
+      <c r="AA29" s="72"/>
+    </row>
+    <row r="30" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A30" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="50">
+        <v>45432</v>
+      </c>
+      <c r="E30" s="51">
+        <v>45448</v>
+      </c>
       <c r="F30" s="63"/>
-      <c r="G30" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H30" s="75"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="75"/>
-      <c r="K30" s="75"/>
-      <c r="L30" s="75"/>
-      <c r="M30" s="75"/>
-      <c r="N30" s="75"/>
-      <c r="O30" s="75"/>
-      <c r="P30" s="75"/>
-      <c r="Q30" s="75"/>
-      <c r="R30" s="75"/>
-      <c r="S30" s="75"/>
-      <c r="T30" s="75"/>
-      <c r="U30" s="74"/>
-      <c r="V30" s="74"/>
-      <c r="W30" s="74"/>
-      <c r="X30" s="74"/>
-      <c r="Y30" s="74"/>
-      <c r="Z30" s="74"/>
-      <c r="AA30" s="74"/>
-    </row>
-    <row r="31" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="63">
+        <f t="shared" ca="1" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="H30" s="101"/>
+      <c r="I30" s="101"/>
+      <c r="J30" s="101"/>
+      <c r="K30" s="101"/>
+      <c r="L30" s="101"/>
+      <c r="M30" s="101"/>
+      <c r="N30" s="101"/>
+      <c r="O30" s="101"/>
+      <c r="P30" s="101"/>
+      <c r="Q30" s="101"/>
+      <c r="R30" s="101"/>
+      <c r="S30" s="101"/>
+      <c r="T30" s="101" t="s">
+        <v>23</v>
+      </c>
+      <c r="U30" s="72"/>
+      <c r="V30" s="72"/>
+      <c r="W30" s="72"/>
+      <c r="X30" s="72"/>
+      <c r="Y30" s="72"/>
+      <c r="Z30" s="72"/>
+      <c r="AA30" s="72"/>
+    </row>
+    <row r="31" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A31" s="22"/>
       <c r="B31" s="40" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
+        <v>45</v>
+      </c>
+      <c r="D31" s="52">
+        <v>45439</v>
+      </c>
+      <c r="E31" s="52">
+        <v>45442</v>
+      </c>
       <c r="F31" s="63"/>
-      <c r="G31" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H31" s="75"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="75"/>
-      <c r="K31" s="75"/>
-      <c r="L31" s="75"/>
-      <c r="M31" s="75"/>
-      <c r="N31" s="75"/>
-      <c r="O31" s="75"/>
-      <c r="P31" s="75"/>
-      <c r="Q31" s="75"/>
-      <c r="R31" s="75"/>
-      <c r="S31" s="75"/>
-      <c r="T31" s="75"/>
-      <c r="U31" s="74"/>
-      <c r="V31" s="74"/>
-      <c r="W31" s="74"/>
-      <c r="X31" s="74"/>
-      <c r="Y31" s="74"/>
-      <c r="Z31" s="74"/>
-      <c r="AA31" s="74"/>
-    </row>
-    <row r="32" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="63">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H31" s="73"/>
+      <c r="I31" s="73"/>
+      <c r="J31" s="73"/>
+      <c r="K31" s="73"/>
+      <c r="L31" s="73"/>
+      <c r="M31" s="94"/>
+      <c r="N31" s="94"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="94"/>
+      <c r="Q31" s="94" t="s">
+        <v>23</v>
+      </c>
+      <c r="R31" s="73"/>
+      <c r="S31" s="73"/>
+      <c r="T31" s="73"/>
+      <c r="U31" s="72"/>
+      <c r="V31" s="72"/>
+      <c r="W31" s="72"/>
+      <c r="X31" s="72"/>
+      <c r="Y31" s="72"/>
+      <c r="Z31" s="72"/>
+      <c r="AA31" s="72"/>
+    </row>
+    <row r="32" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A32" s="22"/>
       <c r="B32" s="40" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
+        <v>45</v>
+      </c>
+      <c r="D32" s="52">
+        <v>45440</v>
+      </c>
+      <c r="E32" s="52">
+        <v>45443</v>
+      </c>
       <c r="F32" s="63"/>
-      <c r="G32" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H32" s="75"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="75"/>
-      <c r="L32" s="75"/>
-      <c r="M32" s="75"/>
-      <c r="N32" s="75"/>
-      <c r="O32" s="75"/>
-      <c r="P32" s="75"/>
-      <c r="Q32" s="75"/>
-      <c r="R32" s="75"/>
-      <c r="S32" s="75"/>
-      <c r="T32" s="75"/>
-      <c r="U32" s="74"/>
-      <c r="V32" s="74"/>
-      <c r="W32" s="74"/>
-      <c r="X32" s="74"/>
-      <c r="Y32" s="74"/>
-      <c r="Z32" s="74"/>
-      <c r="AA32" s="74"/>
-    </row>
-    <row r="33" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="63">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H32" s="73"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="73"/>
+      <c r="K32" s="73"/>
+      <c r="L32" s="73"/>
+      <c r="M32" s="86"/>
+      <c r="N32" s="86"/>
+      <c r="O32" s="86"/>
+      <c r="P32" s="86"/>
+      <c r="Q32" s="86" t="s">
+        <v>23</v>
+      </c>
+      <c r="R32" s="73"/>
+      <c r="S32" s="73"/>
+      <c r="T32" s="73"/>
+      <c r="U32" s="72"/>
+      <c r="V32" s="72"/>
+      <c r="W32" s="72"/>
+      <c r="X32" s="72"/>
+      <c r="Y32" s="72"/>
+      <c r="Z32" s="72"/>
+      <c r="AA32" s="72"/>
+    </row>
+    <row r="33" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A33" s="22"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="52"/>
+      <c r="B33" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="52">
+        <v>45441</v>
+      </c>
+      <c r="E33" s="52">
+        <v>45447</v>
+      </c>
       <c r="F33" s="63"/>
-      <c r="G33" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H33" s="75"/>
-      <c r="I33" s="75"/>
-      <c r="J33" s="75"/>
-      <c r="K33" s="75"/>
-      <c r="L33" s="75"/>
-      <c r="M33" s="75"/>
-      <c r="N33" s="75"/>
-      <c r="O33" s="75"/>
-      <c r="P33" s="75"/>
-      <c r="Q33" s="75"/>
-      <c r="R33" s="75"/>
-      <c r="S33" s="75"/>
-      <c r="T33" s="75"/>
-      <c r="U33" s="74"/>
-      <c r="V33" s="74"/>
-      <c r="W33" s="74"/>
-      <c r="X33" s="74"/>
-      <c r="Y33" s="74"/>
-      <c r="Z33" s="74"/>
-      <c r="AA33" s="74"/>
-    </row>
-    <row r="34" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="54"/>
+      <c r="G33" s="63">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="H33" s="73"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="73"/>
+      <c r="L33" s="73"/>
+      <c r="M33" s="86"/>
+      <c r="N33" s="86"/>
+      <c r="O33" s="86"/>
+      <c r="P33" s="86"/>
+      <c r="Q33" s="86"/>
+      <c r="R33" s="86"/>
+      <c r="S33" s="86" t="s">
+        <v>23</v>
+      </c>
+      <c r="T33" s="73"/>
+      <c r="U33" s="72"/>
+      <c r="V33" s="72"/>
+      <c r="W33" s="72"/>
+      <c r="X33" s="72"/>
+      <c r="Y33" s="72"/>
+      <c r="Z33" s="72"/>
+      <c r="AA33" s="72"/>
+    </row>
+    <row r="34" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A34" s="22"/>
+      <c r="B34" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="52">
+        <v>45442</v>
+      </c>
+      <c r="E34" s="52">
+        <v>45448</v>
+      </c>
       <c r="F34" s="63"/>
-      <c r="G34" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H34" s="75"/>
-      <c r="I34" s="75"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="75"/>
-      <c r="M34" s="75"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="75"/>
-      <c r="P34" s="75"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="75"/>
-      <c r="S34" s="75"/>
-      <c r="T34" s="75"/>
-      <c r="U34" s="74"/>
-      <c r="V34" s="74"/>
-      <c r="W34" s="74"/>
-      <c r="X34" s="74"/>
-      <c r="Y34" s="74"/>
-      <c r="Z34" s="74"/>
-      <c r="AA34" s="74"/>
-    </row>
-    <row r="35" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="22"/>
-      <c r="B35" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H35" s="74"/>
-      <c r="I35" s="74"/>
-      <c r="J35" s="74"/>
-      <c r="K35" s="74"/>
-      <c r="L35" s="74"/>
-      <c r="M35" s="74"/>
-      <c r="N35" s="74"/>
-      <c r="O35" s="74"/>
-      <c r="P35" s="74"/>
-      <c r="Q35" s="74"/>
-      <c r="R35" s="74"/>
-      <c r="S35" s="74"/>
-      <c r="T35" s="74"/>
-      <c r="U35" s="74"/>
-      <c r="V35" s="74"/>
-      <c r="W35" s="74"/>
-      <c r="X35" s="74"/>
-      <c r="Y35" s="74"/>
-      <c r="Z35" s="74"/>
-      <c r="AA35" s="74"/>
-    </row>
-    <row r="36" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="63">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="86"/>
+      <c r="N34" s="86"/>
+      <c r="O34" s="86"/>
+      <c r="P34" s="86"/>
+      <c r="Q34" s="86"/>
+      <c r="R34" s="86"/>
+      <c r="S34" s="86" t="s">
+        <v>23</v>
+      </c>
+      <c r="T34" s="73"/>
+      <c r="U34" s="72"/>
+      <c r="V34" s="72"/>
+      <c r="W34" s="72"/>
+      <c r="X34" s="72"/>
+      <c r="Y34" s="72"/>
+      <c r="Z34" s="72"/>
+      <c r="AA34" s="72"/>
+    </row>
+    <row r="35" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A35" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="35"/>
+      <c r="D35" s="53">
+        <v>45432</v>
+      </c>
+      <c r="E35" s="54">
+        <v>45448</v>
+      </c>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63">
+        <f t="shared" ca="1" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="H35" s="101"/>
+      <c r="I35" s="101"/>
+      <c r="J35" s="101"/>
+      <c r="K35" s="101"/>
+      <c r="L35" s="101"/>
+      <c r="M35" s="101"/>
+      <c r="N35" s="101"/>
+      <c r="O35" s="101"/>
+      <c r="P35" s="101"/>
+      <c r="Q35" s="101"/>
+      <c r="R35" s="101"/>
+      <c r="S35" s="101"/>
+      <c r="T35" s="101" t="s">
+        <v>23</v>
+      </c>
+      <c r="U35" s="72"/>
+      <c r="V35" s="72"/>
+      <c r="W35" s="72"/>
+      <c r="X35" s="72"/>
+      <c r="Y35" s="72"/>
+      <c r="Z35" s="72"/>
+      <c r="AA35" s="72"/>
+    </row>
+    <row r="36" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A36" s="22"/>
       <c r="B36" s="41" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
+        <v>26</v>
+      </c>
+      <c r="D36" s="55">
+        <v>45432</v>
+      </c>
+      <c r="E36" s="55">
+        <v>45448</v>
+      </c>
       <c r="F36" s="13"/>
-      <c r="G36" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="G36" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>17</v>
       </c>
       <c r="H36" s="74"/>
       <c r="I36" s="74"/>
@@ -3322,337 +3637,432 @@
       <c r="Q36" s="74"/>
       <c r="R36" s="74"/>
       <c r="S36" s="74"/>
-      <c r="T36" s="74"/>
-      <c r="U36" s="74"/>
-      <c r="V36" s="74"/>
-      <c r="W36" s="74"/>
-      <c r="X36" s="74"/>
-      <c r="Y36" s="74"/>
-      <c r="Z36" s="74"/>
-      <c r="AA36" s="74"/>
-    </row>
-    <row r="37" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T36" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="U36" s="72"/>
+      <c r="V36" s="72"/>
+      <c r="W36" s="72"/>
+      <c r="X36" s="72"/>
+      <c r="Y36" s="72"/>
+      <c r="Z36" s="72"/>
+      <c r="AA36" s="72"/>
+    </row>
+    <row r="37" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A37" s="22"/>
       <c r="B37" s="41" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
+        <v>65</v>
+      </c>
+      <c r="D37" s="55">
+        <v>45443</v>
+      </c>
+      <c r="E37" s="55">
+        <v>45448</v>
+      </c>
       <c r="F37" s="13"/>
-      <c r="G37" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="74"/>
-      <c r="N37" s="74"/>
-      <c r="O37" s="74"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="74"/>
-      <c r="S37" s="74"/>
-      <c r="T37" s="74"/>
-      <c r="U37" s="74"/>
-      <c r="V37" s="74"/>
-      <c r="W37" s="74"/>
-      <c r="X37" s="74"/>
-      <c r="Y37" s="74"/>
-      <c r="Z37" s="74"/>
-      <c r="AA37" s="74"/>
-    </row>
-    <row r="38" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="H37" s="72"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="72"/>
+      <c r="N37" s="72"/>
+      <c r="O37" s="72"/>
+      <c r="P37" s="72"/>
+      <c r="Q37" s="76"/>
+      <c r="R37" s="76"/>
+      <c r="S37" s="76"/>
+      <c r="T37" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="U37" s="72"/>
+      <c r="V37" s="72"/>
+      <c r="W37" s="72"/>
+      <c r="X37" s="72"/>
+      <c r="Y37" s="72"/>
+      <c r="Z37" s="72"/>
+      <c r="AA37" s="72"/>
+    </row>
+    <row r="38" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A38" s="22"/>
       <c r="B38" s="41" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C38" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
+      <c r="D38" s="55">
+        <v>45447</v>
+      </c>
+      <c r="E38" s="55">
+        <v>45448</v>
+      </c>
       <c r="F38" s="13"/>
-      <c r="G38" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H38" s="74"/>
-      <c r="I38" s="74"/>
-      <c r="J38" s="74"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="74"/>
-      <c r="M38" s="74"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="74"/>
-      <c r="P38" s="74"/>
-      <c r="Q38" s="74"/>
-      <c r="R38" s="74"/>
-      <c r="S38" s="74"/>
-      <c r="T38" s="74"/>
-      <c r="U38" s="74"/>
-      <c r="V38" s="74"/>
-      <c r="W38" s="74"/>
-      <c r="X38" s="74"/>
-      <c r="Y38" s="74"/>
-      <c r="Z38" s="74"/>
-      <c r="AA38" s="74"/>
-    </row>
-    <row r="39" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G38" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="H38" s="72"/>
+      <c r="I38" s="72"/>
+      <c r="J38" s="72"/>
+      <c r="K38" s="72"/>
+      <c r="L38" s="72"/>
+      <c r="M38" s="72"/>
+      <c r="N38" s="73"/>
+      <c r="O38" s="73"/>
+      <c r="P38" s="73"/>
+      <c r="Q38" s="73"/>
+      <c r="R38" s="72"/>
+      <c r="S38" s="99"/>
+      <c r="T38" s="99" t="s">
+        <v>23</v>
+      </c>
+      <c r="U38" s="72"/>
+      <c r="V38" s="72"/>
+      <c r="W38" s="72"/>
+      <c r="X38" s="72"/>
+      <c r="Y38" s="72"/>
+      <c r="Z38" s="72"/>
+      <c r="AA38" s="72"/>
+    </row>
+    <row r="39" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A39" s="22"/>
       <c r="B39" s="41" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
+        <v>33</v>
+      </c>
+      <c r="D39" s="55">
+        <v>45448</v>
+      </c>
+      <c r="E39" s="55">
+        <v>45448</v>
+      </c>
       <c r="F39" s="13"/>
-      <c r="G39" s="13" t="str">
-        <f t="shared" si="3"/>
+      <c r="G39" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H39" s="72"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="72"/>
+      <c r="K39" s="72"/>
+      <c r="L39" s="72"/>
+      <c r="M39" s="72"/>
+      <c r="N39" s="72"/>
+      <c r="O39" s="72"/>
+      <c r="P39" s="72"/>
+      <c r="Q39" s="72"/>
+      <c r="R39" s="72"/>
+      <c r="S39" s="99"/>
+      <c r="T39" s="99" t="s">
+        <v>23</v>
+      </c>
+      <c r="U39" s="72"/>
+      <c r="V39" s="72"/>
+      <c r="W39" s="72"/>
+      <c r="X39" s="72"/>
+      <c r="Y39" s="72"/>
+      <c r="Z39" s="72"/>
+      <c r="AA39" s="72"/>
+    </row>
+    <row r="40" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A40" s="22"/>
+      <c r="B40" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="55">
+        <v>45449</v>
+      </c>
+      <c r="E40" s="55">
+        <v>45448</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="72"/>
+      <c r="I40" s="72"/>
+      <c r="J40" s="72"/>
+      <c r="K40" s="72"/>
+      <c r="L40" s="72"/>
+      <c r="M40" s="72"/>
+      <c r="N40" s="72"/>
+      <c r="O40" s="72"/>
+      <c r="P40" s="72"/>
+      <c r="Q40" s="72"/>
+      <c r="R40" s="72"/>
+      <c r="S40" s="100"/>
+      <c r="T40" s="100" t="s">
+        <v>23</v>
+      </c>
+      <c r="U40" s="72"/>
+      <c r="V40" s="72"/>
+      <c r="W40" s="72"/>
+      <c r="X40" s="72"/>
+      <c r="Y40" s="72"/>
+      <c r="Z40" s="72"/>
+      <c r="AA40" s="72"/>
+    </row>
+    <row r="41" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A41" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="66"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63" t="str">
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="H39" s="74"/>
-      <c r="I39" s="74"/>
-      <c r="J39" s="74"/>
-      <c r="K39" s="74"/>
-      <c r="L39" s="74"/>
-      <c r="M39" s="74"/>
-      <c r="N39" s="74"/>
-      <c r="O39" s="74"/>
-      <c r="P39" s="74"/>
-      <c r="Q39" s="74"/>
-      <c r="R39" s="74"/>
-      <c r="S39" s="74"/>
-      <c r="T39" s="74"/>
-      <c r="U39" s="74"/>
-      <c r="V39" s="74"/>
-      <c r="W39" s="74"/>
-      <c r="X39" s="74"/>
-      <c r="Y39" s="74"/>
-      <c r="Z39" s="74"/>
-      <c r="AA39" s="74"/>
-    </row>
-    <row r="40" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" s="66"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="68"/>
-      <c r="F40" s="63"/>
-      <c r="G40" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H40" s="75"/>
-      <c r="I40" s="75"/>
-      <c r="J40" s="75"/>
-      <c r="K40" s="75"/>
-      <c r="L40" s="75"/>
-      <c r="M40" s="75"/>
-      <c r="N40" s="75"/>
-      <c r="O40" s="75"/>
-      <c r="P40" s="75"/>
-      <c r="Q40" s="75"/>
-      <c r="R40" s="75"/>
-      <c r="S40" s="75"/>
-      <c r="T40" s="75"/>
-      <c r="U40" s="74"/>
-      <c r="V40" s="74"/>
-      <c r="W40" s="74"/>
-      <c r="X40" s="74"/>
-      <c r="Y40" s="74"/>
-      <c r="Z40" s="74"/>
-      <c r="AA40" s="74"/>
-    </row>
-    <row r="41" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="22"/>
-      <c r="B41" s="69" t="s">
-        <v>72</v>
-      </c>
-      <c r="C41" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="74"/>
-      <c r="J41" s="74"/>
-      <c r="K41" s="74"/>
-      <c r="L41" s="74"/>
-      <c r="M41" s="74"/>
-      <c r="N41" s="74"/>
-      <c r="O41" s="74"/>
-      <c r="P41" s="74"/>
-      <c r="Q41" s="74"/>
-      <c r="R41" s="74"/>
-      <c r="S41" s="74"/>
-      <c r="T41" s="74"/>
-      <c r="U41" s="74"/>
-      <c r="V41" s="74"/>
-      <c r="W41" s="74"/>
-      <c r="X41" s="74"/>
-      <c r="Y41" s="74"/>
-      <c r="Z41" s="74"/>
-      <c r="AA41" s="74"/>
-    </row>
-    <row r="42" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H41" s="73"/>
+      <c r="I41" s="73"/>
+      <c r="J41" s="73"/>
+      <c r="K41" s="73"/>
+      <c r="L41" s="73"/>
+      <c r="M41" s="73"/>
+      <c r="N41" s="73"/>
+      <c r="O41" s="73"/>
+      <c r="P41" s="73"/>
+      <c r="Q41" s="73"/>
+      <c r="R41" s="73"/>
+      <c r="S41" s="73"/>
+      <c r="T41" s="73"/>
+      <c r="U41" s="72"/>
+      <c r="V41" s="72"/>
+      <c r="W41" s="72"/>
+      <c r="X41" s="72"/>
+      <c r="Y41" s="72"/>
+      <c r="Z41" s="72"/>
+      <c r="AA41" s="72"/>
+    </row>
+    <row r="42" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A42" s="22"/>
-      <c r="B42" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
+      <c r="B42" s="88" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="89" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="74"/>
-      <c r="J42" s="74"/>
-      <c r="K42" s="74"/>
-      <c r="L42" s="74"/>
-      <c r="M42" s="74"/>
-      <c r="N42" s="74"/>
-      <c r="O42" s="74"/>
-      <c r="P42" s="74"/>
-      <c r="Q42" s="74"/>
-      <c r="R42" s="74"/>
-      <c r="S42" s="74"/>
-      <c r="T42" s="74"/>
-      <c r="U42" s="74"/>
-      <c r="V42" s="74"/>
-      <c r="W42" s="74"/>
-      <c r="X42" s="74"/>
-      <c r="Y42" s="74"/>
-      <c r="Z42" s="74"/>
-      <c r="AA42" s="74"/>
-    </row>
-    <row r="43" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="72"/>
+      <c r="N42" s="72"/>
+      <c r="O42" s="72"/>
+      <c r="P42" s="72"/>
+      <c r="Q42" s="72"/>
+      <c r="R42" s="72"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
+      <c r="W42" s="72"/>
+      <c r="X42" s="72"/>
+      <c r="Y42" s="72"/>
+      <c r="Z42" s="72"/>
+      <c r="AA42" s="72"/>
+    </row>
+    <row r="43" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A43" s="22"/>
-      <c r="B43" s="69" t="s">
+      <c r="B43" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="70" t="s">
-        <v>31</v>
-      </c>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
+      <c r="C43" s="89" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
-      <c r="H43" s="74"/>
-      <c r="I43" s="74"/>
-      <c r="J43" s="74"/>
-      <c r="K43" s="74"/>
-      <c r="L43" s="74"/>
-      <c r="M43" s="74"/>
-      <c r="N43" s="74"/>
-      <c r="O43" s="74"/>
-      <c r="P43" s="74"/>
-      <c r="Q43" s="74"/>
-      <c r="R43" s="74"/>
-      <c r="S43" s="74"/>
-      <c r="T43" s="74"/>
-      <c r="U43" s="74"/>
-      <c r="V43" s="74"/>
-      <c r="W43" s="74"/>
-      <c r="X43" s="74"/>
-      <c r="Y43" s="74"/>
-      <c r="Z43" s="74"/>
-      <c r="AA43" s="74"/>
-    </row>
-    <row r="44" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="42"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="56"/>
+      <c r="H43" s="72"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="72"/>
+      <c r="K43" s="72"/>
+      <c r="L43" s="72"/>
+      <c r="M43" s="72"/>
+      <c r="N43" s="72"/>
+      <c r="O43" s="72"/>
+      <c r="P43" s="72"/>
+      <c r="Q43" s="72"/>
+      <c r="R43" s="72"/>
+      <c r="S43" s="72"/>
+      <c r="T43" s="72"/>
+      <c r="U43" s="72"/>
+      <c r="V43" s="72"/>
+      <c r="W43" s="72"/>
+      <c r="X43" s="72"/>
+      <c r="Y43" s="72"/>
+      <c r="Z43" s="72"/>
+      <c r="AA43" s="72"/>
+    </row>
+    <row r="44" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A44" s="22"/>
+      <c r="B44" s="88" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="89" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
       <c r="F44" s="13"/>
-      <c r="G44" s="13" t="str">
-        <f t="shared" si="3"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="72"/>
+      <c r="I44" s="72"/>
+      <c r="J44" s="72"/>
+      <c r="K44" s="72"/>
+      <c r="L44" s="72"/>
+      <c r="M44" s="72"/>
+      <c r="N44" s="72"/>
+      <c r="O44" s="72"/>
+      <c r="P44" s="72"/>
+      <c r="Q44" s="72"/>
+      <c r="R44" s="72"/>
+      <c r="S44" s="72"/>
+      <c r="T44" s="72"/>
+      <c r="U44" s="72"/>
+      <c r="V44" s="72"/>
+      <c r="W44" s="72"/>
+      <c r="X44" s="72"/>
+      <c r="Y44" s="72"/>
+      <c r="Z44" s="72"/>
+      <c r="AA44" s="72"/>
+    </row>
+    <row r="45" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A45" s="22"/>
+      <c r="B45" s="88" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="72"/>
+      <c r="I45" s="72"/>
+      <c r="J45" s="72"/>
+      <c r="K45" s="72"/>
+      <c r="L45" s="72"/>
+      <c r="M45" s="72"/>
+      <c r="N45" s="72"/>
+      <c r="O45" s="72"/>
+      <c r="P45" s="72"/>
+      <c r="Q45" s="72"/>
+      <c r="R45" s="72"/>
+      <c r="S45" s="72"/>
+      <c r="T45" s="72"/>
+      <c r="U45" s="72"/>
+      <c r="V45" s="72"/>
+      <c r="W45" s="72"/>
+      <c r="X45" s="72"/>
+      <c r="Y45" s="72"/>
+      <c r="Z45" s="72"/>
+      <c r="AA45" s="72"/>
+    </row>
+    <row r="46" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A46" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="42"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13" t="str">
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="H44" s="74"/>
-      <c r="I44" s="74"/>
-      <c r="J44" s="74"/>
-      <c r="K44" s="74"/>
-      <c r="L44" s="74"/>
-      <c r="M44" s="74"/>
-      <c r="N44" s="74"/>
-      <c r="O44" s="74"/>
-      <c r="P44" s="74"/>
-      <c r="Q44" s="74"/>
-      <c r="R44" s="74"/>
-      <c r="S44" s="74"/>
-      <c r="T44" s="74"/>
-      <c r="U44" s="74"/>
-      <c r="V44" s="74"/>
-      <c r="W44" s="74"/>
-      <c r="X44" s="74"/>
-      <c r="Y44" s="74"/>
-      <c r="Z44" s="74"/>
-      <c r="AA44" s="74"/>
-    </row>
-    <row r="45" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C45" s="19"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20" t="str">
-        <f t="shared" si="3"/>
+      <c r="H46" s="72"/>
+      <c r="I46" s="72"/>
+      <c r="J46" s="72"/>
+      <c r="K46" s="72"/>
+      <c r="L46" s="72"/>
+      <c r="M46" s="72"/>
+      <c r="N46" s="72"/>
+      <c r="O46" s="72"/>
+      <c r="P46" s="72"/>
+      <c r="Q46" s="72"/>
+      <c r="R46" s="72"/>
+      <c r="S46" s="72"/>
+      <c r="T46" s="72"/>
+      <c r="U46" s="72"/>
+      <c r="V46" s="72"/>
+      <c r="W46" s="72"/>
+      <c r="X46" s="72"/>
+      <c r="Y46" s="72"/>
+      <c r="Z46" s="72"/>
+      <c r="AA46" s="72"/>
+    </row>
+    <row r="47" spans="1:27" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A47" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" s="19"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20" t="str">
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="H45" s="79"/>
-      <c r="I45" s="79"/>
-      <c r="J45" s="79"/>
-      <c r="K45" s="79"/>
-      <c r="L45" s="79"/>
-      <c r="M45" s="79"/>
-      <c r="N45" s="79"/>
-      <c r="O45" s="79"/>
-      <c r="P45" s="79"/>
-      <c r="Q45" s="79"/>
-      <c r="R45" s="79"/>
-      <c r="S45" s="79"/>
-      <c r="T45" s="79"/>
-      <c r="U45" s="79"/>
-      <c r="V45" s="79"/>
-      <c r="W45" s="79"/>
-      <c r="X45" s="79"/>
-      <c r="Y45" s="79"/>
-      <c r="Z45" s="79"/>
-      <c r="AA45" s="79"/>
-    </row>
-    <row r="46" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F46" s="6"/>
-    </row>
-    <row r="47" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="11"/>
-      <c r="E47" s="24"/>
-    </row>
-    <row r="48" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="12"/>
+      <c r="H47" s="77"/>
+      <c r="I47" s="77"/>
+      <c r="J47" s="77"/>
+      <c r="K47" s="77"/>
+      <c r="L47" s="77"/>
+      <c r="M47" s="77"/>
+      <c r="N47" s="77"/>
+      <c r="O47" s="77"/>
+      <c r="P47" s="77"/>
+      <c r="Q47" s="77"/>
+      <c r="R47" s="77"/>
+      <c r="S47" s="77"/>
+      <c r="T47" s="77"/>
+      <c r="U47" s="77"/>
+      <c r="V47" s="77"/>
+      <c r="W47" s="77"/>
+      <c r="X47" s="77"/>
+      <c r="Y47" s="77"/>
+      <c r="Z47" s="77"/>
+      <c r="AA47" s="77"/>
+    </row>
+    <row r="48" spans="1:27" ht="30" customHeight="1">
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="3:5" ht="30" customHeight="1">
+      <c r="C49" s="11"/>
+      <c r="E49" s="24"/>
+    </row>
+    <row r="50" spans="3:5" ht="30" customHeight="1">
+      <c r="C50" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3662,37 +4072,37 @@
     <mergeCell ref="R4:V4"/>
     <mergeCell ref="W4:AA4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:K7 M5:P7 R5:U7 W5:Z7 H44:K45 M44:P45 R44:U45 W44:Z45">
+  <conditionalFormatting sqref="H5:K7 M5:P7 R5:U7 W5:Z7 H46:K47 M46:P47 R46:U47 W46:Z47">
     <cfRule type="expression" dxfId="6" priority="35">
       <formula>AND(TODAY()&gt;=H$5,TODAY()&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:K7 M7:P7 R7:U7 W7:Z7 H44:K45 M44:P45 R44:U45 W44:Z45">
+  <conditionalFormatting sqref="H7:K7 M7:P7 R7:U7 W7:Z7 H46:K47 M46:P47 R46:U47 W46:Z47">
     <cfRule type="expression" dxfId="5" priority="30" stopIfTrue="1">
       <formula>AND(task_end&gt;=H$5,task_start&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:AA7 H44:AA45">
+  <conditionalFormatting sqref="H7:AA7 H46:AA47">
     <cfRule type="expression" dxfId="4" priority="29">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7 Q7 AA7 L44:L45 Q44:Q45 V44:V45 AA44:AA45 V7">
-    <cfRule type="expression" dxfId="3" priority="44" stopIfTrue="1">
+  <conditionalFormatting sqref="L5:L7 Q5:Q7 L46:L47 Q46:Q47 V46:V47 AA46:AA47">
+    <cfRule type="expression" dxfId="3" priority="38">
+      <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L7 Q7 L46:L47 Q46:Q47 V46:V47 AA46:AA47 V7 AA7">
+    <cfRule type="expression" dxfId="2" priority="44" stopIfTrue="1">
       <formula>AND(task_end&gt;=L$5,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V5:V7">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(TODAY()&gt;=V$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA5 L5:L7 Q5:Q7 AA7 L44:L45 Q44:Q45 V44:V45 AA44:AA45">
-    <cfRule type="expression" dxfId="1" priority="38">
-      <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA6">
+  <conditionalFormatting sqref="AA5:AA7">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(TODAY()&gt;=AA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
@@ -3713,23 +4123,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100CE8683845CA09544BDD5D2CFA119F453" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="25e64108eeebe26551eee07707bcd7de">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="490ce474-600e-4e79-85eb-56e37e2f143b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="23adf563ecffdbcf6d9713f65d527ff9" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100CE8683845CA09544BDD5D2CFA119F453" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a3e0b86ddfb5888667688fb444501dea">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="490ce474-600e-4e79-85eb-56e37e2f143b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2da774dfbd938cc3f071244fda822046" ns2:_="">
     <xsd:import namespace="490ce474-600e-4e79-85eb-56e37e2f143b"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -3741,6 +4136,11 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3767,6 +4167,35 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="9b687ba5-7c2c-441d-a210-8f2e7a637e62" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -3871,37 +4300,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="490ce474-600e-4e79-85eb-56e37e2f143b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{246EE659-F553-4E88-8595-FF430B089FFB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3471B813-2B12-46F0-BD03-DECCBFECE95B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="490ce474-600e-4e79-85eb-56e37e2f143b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}"/>
 </file>
</xml_diff>